<commit_message>
updates to buzzi... still lot of work to do - next step: estimates on each country
</commit_message>
<xml_diff>
--- a/Buzzi SpA/UCM_model.xlsx
+++ b/Buzzi SpA/UCM_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/equity_research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/equity_research/Buzzi SpA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2119" documentId="11_AD4D5CB4E552A5DACE1C6418181876DE5ADEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51EF2F90-440D-4031-BC5F-A32C850A9E43}"/>
+  <xr:revisionPtr revIDLastSave="2641" documentId="11_AD4D5CB4E552A5DACE1C6418181876DE5ADEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{887355E6-4967-40B3-9B83-AA6D2ACE23A1}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assumptions" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,6 @@
     <sheet name="income_statement" sheetId="1" r:id="rId4"/>
     <sheet name="balance_sheet" sheetId="7" r:id="rId5"/>
     <sheet name="cash_flow_statement" sheetId="8" r:id="rId6"/>
-    <sheet name="forecast" sheetId="3" r:id="rId7"/>
-    <sheet name="multiples_comparables" sheetId="5" r:id="rId8"/>
-    <sheet name="sensitivity_analysis" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="209">
   <si>
     <t>Other operating revenues</t>
   </si>
@@ -563,9 +560,6 @@
     <t>% of sales</t>
   </si>
   <si>
-    <t>margin</t>
-  </si>
-  <si>
     <t>D&amp;A</t>
   </si>
   <si>
@@ -602,9 +596,6 @@
     <t>EBIT to cash conversion</t>
   </si>
   <si>
-    <t>g (expected from buzzi - based on inflation)</t>
-  </si>
-  <si>
     <t>WACC (estimated by Buzzi)</t>
   </si>
   <si>
@@ -671,7 +662,49 @@
     <t>D/(E+D)</t>
   </si>
   <si>
-    <t>BTP 10y</t>
+    <t>26-28E CAGR</t>
+  </si>
+  <si>
+    <t>growth rate</t>
+  </si>
+  <si>
+    <t>CAGR revenues</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>19-23 AVG</t>
+  </si>
+  <si>
+    <t>% EBITDA</t>
+  </si>
+  <si>
+    <t>margin EBITDA</t>
+  </si>
+  <si>
+    <t>BUND 10y</t>
+  </si>
+  <si>
+    <t>Growth revenues based on CAGR</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>terminal growth rate</t>
+  </si>
+  <si>
+    <t>19-23 AVG margin</t>
+  </si>
+  <si>
+    <t>26-28E AVG margin</t>
+  </si>
+  <si>
+    <t>EBITDA,EBIT, Net Profit margin on sales</t>
+  </si>
+  <si>
+    <t>All the margins are based on 2023 margins reduced each year to get closer to the historical average</t>
   </si>
 </sst>
 </file>
@@ -686,9 +719,9 @@
     <numFmt numFmtId="167" formatCode="#,##0.0\ &quot;€&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0\ &quot;€&quot;;[Red]\-#,##0.0\ &quot;€&quot;"/>
-    <numFmt numFmtId="176" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="185" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0\ &quot;€&quot;;[Red]\-#,##0.0\ &quot;€&quot;"/>
+    <numFmt numFmtId="171" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -966,23 +999,18 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -994,13 +1022,9 @@
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1011,8 +1035,6 @@
     <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1020,25 +1042,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -1058,6 +1089,19 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="10" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
@@ -1174,9 +1218,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{67E96F2F-D7BF-4118-9F56-73AA47E3F838}">
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="lastTotalCell" dxfId="10"/>
+      <tableStyleElement type="totalRow" dxfId="13"/>
+      <tableStyleElement type="firstRowStripe" dxfId="12"/>
+      <tableStyleElement type="lastTotalCell" dxfId="11"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1320,23 +1364,23 @@
     <v>4</v>
     <v>Finance</v>
     <v>5</v>
-    <v>51.2</v>
+    <v>47</v>
     <v>192626100</v>
     <v>0.96540000000000004</v>
-    <v>10072310000</v>
-    <v>54.35</v>
+    <v>9011052000</v>
+    <v>47.44</v>
     <v>Buzzi Unicem S.p.A., precedentemente nota come Buzzi Unicem S.p.A. - Senza Vincoli di Rappresentazione Grafica, è una società con sede in Italia impegnata nella produzione di materiali da costruzione. La Società è principalmente attiva nella produzione, distribuzione e vendita di cemento, aggregati naturali e preconfezionati. Le attività della Società si svolgono principalmente in Italia, Stati Uniti, Germania, Lussemburgo, Paesi Bassi, Polonia, Repubblica Ceca, Slovacchia, Ucraina, Russia e Messico. Al 31 dicembre 2011, la Società disponeva di una capacità produttiva complessiva di circa 44 milioni di tonnellate di cemento all'anno, e gestiva 39 cementifici, 558 impianti di calcestruzzo preconfezionati, 37 cave di aggregati e 41 terminali.</v>
     <v>9843</v>
     <v>Deutsche Boerse AG</v>
     <v>XFRA</v>
     <v>0</v>
-    <v>51.9</v>
-    <v>50.6</v>
+    <v>47.66</v>
+    <v>45.78</v>
     <v>Buzzi SpA</v>
     <v>Buzzi SpA</v>
-    <v>45737.878472222219</v>
-    <v>9.7872000000000003</v>
-    <v>50.6</v>
+    <v>45744.878472222219</v>
+    <v>8.8549000000000007</v>
+    <v>45.78</v>
     <v>Via Luigi Buzzi, 6, CASALE MONFERRATO, ALESSANDRIA, 15033 IT</v>
     <v>Construction Materials</v>
     <v>XFRA</v>
@@ -1344,10 +1388,10 @@
     <v>Azionario</v>
     <v>Buzzi SpA (XFRA:UCM)</v>
     <v>EUR</v>
-    <v>-3.75</v>
-    <v>-6.8997000000000003E-2</v>
-    <v>105</v>
-    <v>822020</v>
+    <v>-1.66</v>
+    <v>-3.4992000000000002E-2</v>
+    <v>1</v>
+    <v>639790</v>
   </rv>
   <rv s="2">
     <v>1</v>
@@ -1661,22 +1705,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F68A0CF-6F64-40CD-8BBD-91947DC4B1B7}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
-  <autoFilter ref="A1:F19" xr:uid="{7F68A0CF-6F64-40CD-8BBD-91947DC4B1B7}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F68A0CF-6F64-40CD-8BBD-91947DC4B1B7}" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9">
+  <autoFilter ref="A1:G19" xr:uid="{7F68A0CF-6F64-40CD-8BBD-91947DC4B1B7}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A61A545-83B0-4348-9AB9-7BDEB543ECFC}" name="(thousands of euro)" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{B64D4814-B95E-4268-B203-76CEA43ED831}" name="2019" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{DC75388F-3B36-4C54-850E-D083A3088F7D}" name="2020" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{FFB7C7D8-2563-4878-B86E-54C2610F4C1D}" name="2021" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{6BB45C77-A449-43E3-8CA9-6CDE423FC41F}" name="2022" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{039EB9D4-DBC4-49DC-8CCD-3133FBBCDEF6}" name="2023" dataDxfId="2"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{8A61A545-83B0-4348-9AB9-7BDEB543ECFC}" name="(thousands of euro)" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{B64D4814-B95E-4268-B203-76CEA43ED831}" name="2019" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DC75388F-3B36-4C54-850E-D083A3088F7D}" name="2020" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{FFB7C7D8-2563-4878-B86E-54C2610F4C1D}" name="2021" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6BB45C77-A449-43E3-8CA9-6CDE423FC41F}" name="2022" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{039EB9D4-DBC4-49DC-8CCD-3133FBBCDEF6}" name="2023" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{737B6C0B-8A49-4074-9C18-7D28056B559D}" name="2024" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1945,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B04DC5-20A4-4624-A7FC-AA74A3379BBC}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1962,62 +2008,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="92"/>
-      <c r="B1" s="93" t="s">
+      <c r="A1" s="85"/>
+      <c r="B1" s="86" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="87" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="E1" s="88" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="94" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="95" t="s">
-        <v>189</v>
-      </c>
-      <c r="F1" s="96" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="97" t="e" vm="1">
+      <c r="A2" s="90" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B2" s="98" cm="1">
+      <c r="B2" s="91" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_FV(A2,"Azioni in circolazione",TRUE)</f>
         <v>192626100</v>
       </c>
-      <c r="C2" s="99" cm="1">
+      <c r="C2" s="92" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_FV(A2,"Capitalizzazione di mercato",TRUE)</f>
-        <v>10072310000</v>
-      </c>
-      <c r="D2" s="99" cm="1">
+        <v>9011052000</v>
+      </c>
+      <c r="D2" s="92" cm="1">
         <f t="array" aca="1" ref="D2" ca="1">_FV(A2,"Prezzo")</f>
-        <v>50.6</v>
-      </c>
-      <c r="E2" s="100" cm="1">
+        <v>45.78</v>
+      </c>
+      <c r="E2" s="93" cm="1">
         <f t="array" aca="1" ref="E2" ca="1">_FV(A2,"P/U",TRUE)</f>
-        <v>9.7872000000000003</v>
-      </c>
-      <c r="F2" s="101" cm="1">
+        <v>8.8549000000000007</v>
+      </c>
+      <c r="F2" s="94" cm="1">
         <f t="array" aca="1" ref="F2" ca="1">_FV(A2,"Beta")</f>
         <v>0.96540000000000004</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="78">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="B4" s="50">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B5" s="50">
         <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2027,52 +2101,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E97210-359B-40D0-B5CA-83EFA2834E49}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.41796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="12.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.41796875" customWidth="1"/>
+    <col min="2" max="2" width="12.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.5234375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.20703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.9453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:11" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="57" t="s">
         <v>157</v>
       </c>
       <c r="B1" s="57">
         <v>2023</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="67" t="s">
         <v>134</v>
       </c>
-      <c r="H1" s="69" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="103" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="H1" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="95" t="s">
+        <v>205</v>
+      </c>
+      <c r="K1" s="95" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>121</v>
       </c>
@@ -2081,1092 +2162,1236 @@
         <v>4317489</v>
       </c>
       <c r="C2" s="14">
-        <f>B2*(1+highlights!$B$2)</f>
+        <f>B2*(1+C3)</f>
         <v>4645435.5256781038</v>
       </c>
       <c r="D2" s="14">
-        <f>C2*(1+highlights!$B$2)</f>
-        <v>4998292.1145212408</v>
+        <f t="shared" ref="D2:G2" si="0">C2*(1+D3)</f>
+        <v>4951837.7592644598</v>
       </c>
       <c r="E2" s="14">
-        <f>D2*(1+highlights!$B$2)</f>
-        <v>5377950.8775850264</v>
+        <f t="shared" si="0"/>
+        <v>5278449.5788471699</v>
       </c>
       <c r="F2" s="14">
-        <f>E2*(1+highlights!$B$2)</f>
-        <v>5786447.6463252632</v>
+        <f t="shared" si="0"/>
+        <v>5626603.9621965438</v>
       </c>
       <c r="G2" s="14">
-        <f>F2*(1+highlights!$B$2)</f>
-        <v>6225972.8892686982</v>
+        <f t="shared" si="0"/>
+        <v>5997721.8072281368</v>
       </c>
       <c r="H2" s="66">
         <f>highlights!B2</f>
         <v>7.5957698022647735E-2</v>
       </c>
-      <c r="I2" s="62">
+      <c r="I2" s="66">
         <f>(G2/B2)^(1/5)-1</f>
+        <v>6.7950235002587789E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="69" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="98">
+        <f>$H$2</f>
         <v>7.5957698022647735E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
+      <c r="D3" s="98">
+        <f>$H$2-assumptions!$B$4/5</f>
+        <v>6.595769802264774E-2</v>
+      </c>
+      <c r="E3" s="98">
+        <f>$H$2-assumptions!$B$4/5</f>
+        <v>6.595769802264774E-2</v>
+      </c>
+      <c r="F3" s="98">
+        <f>$H$2-assumptions!$B$4/5</f>
+        <v>6.595769802264774E-2</v>
+      </c>
+      <c r="G3" s="98">
+        <f>$H$2-assumptions!$B$4/5</f>
+        <v>6.595769802264774E-2</v>
+      </c>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="14">
+        <f>income_statement!F9</f>
+        <v>1243215</v>
+      </c>
+      <c r="C4" s="68">
+        <f>C2*C5</f>
+        <v>1337646.7495472261</v>
+      </c>
+      <c r="D4" s="68">
+        <f t="shared" ref="D4:G4" si="1">D2*D5</f>
+        <v>1391211.9855999872</v>
+      </c>
+      <c r="E4" s="68">
+        <f t="shared" si="1"/>
+        <v>1446023.9785797491</v>
+      </c>
+      <c r="F4" s="68">
+        <f t="shared" si="1"/>
+        <v>1502014.1637570441</v>
+      </c>
+      <c r="G4" s="68">
+        <f t="shared" si="1"/>
+        <v>1559099.5077452739</v>
+      </c>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66">
+        <f>(G4/B4)^(1/5)-1</f>
+        <v>4.6322389542504006E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="70">
+        <f>ABS(B4)/$B$2</f>
+        <v>0.28794862013545375</v>
+      </c>
+      <c r="C5" s="70">
+        <f>B5</f>
+        <v>0.28794862013545375</v>
+      </c>
+      <c r="D5" s="70">
+        <f>C5-0.007</f>
+        <v>0.28094862013545374</v>
+      </c>
+      <c r="E5" s="70">
+        <f t="shared" ref="E5:G5" si="2">D5-0.007</f>
+        <v>0.27394862013545374</v>
+      </c>
+      <c r="F5" s="70">
+        <f t="shared" si="2"/>
+        <v>0.26694862013545373</v>
+      </c>
+      <c r="G5" s="70">
+        <f t="shared" si="2"/>
+        <v>0.25994862013545372</v>
+      </c>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="70">
+        <f>highlights!H12</f>
+        <v>0.24161314227219205</v>
+      </c>
+      <c r="K5" s="70">
+        <f>AVERAGE(C5:G5)</f>
+        <v>0.27394862013545374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="14">
+        <f>income_statement!F12</f>
+        <v>984790</v>
+      </c>
+      <c r="C6" s="68">
+        <f>C2*C7</f>
+        <v>1059592.3814357233</v>
+      </c>
+      <c r="D6" s="68">
+        <f t="shared" ref="D6:G6" si="3">D2*D7</f>
+        <v>1094817.7914427076</v>
+      </c>
+      <c r="E6" s="68">
+        <f t="shared" si="3"/>
+        <v>1130080.3056685778</v>
+      </c>
+      <c r="F6" s="68">
+        <f t="shared" si="3"/>
+        <v>1165231.5734758314</v>
+      </c>
+      <c r="G6" s="68">
+        <f t="shared" si="3"/>
+        <v>1200103.5130750081</v>
+      </c>
+      <c r="H6" s="66">
+        <f>(highlights!F15/highlights!B15)^(1/4)-1</f>
+        <v>0.20425717756209383</v>
+      </c>
+      <c r="I6" s="66">
+        <f>(G6/B6)^(1/5)-1</f>
+        <v>4.0339325540836635E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="70">
+        <f>dcf!B6/dcf!B2</f>
+        <v>0.2280932273365375</v>
+      </c>
+      <c r="C7" s="70">
+        <f>B7</f>
+        <v>0.2280932273365375</v>
+      </c>
+      <c r="D7" s="70">
+        <f>C7-0.007</f>
+        <v>0.2210932273365375</v>
+      </c>
+      <c r="E7" s="70">
+        <f t="shared" ref="E7:G7" si="4">D7-0.007</f>
+        <v>0.21409322733653749</v>
+      </c>
+      <c r="F7" s="70">
+        <f t="shared" si="4"/>
+        <v>0.20709322733653748</v>
+      </c>
+      <c r="G7" s="70">
+        <f t="shared" si="4"/>
+        <v>0.20009322733653748</v>
+      </c>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="102">
+        <f>highlights!H16</f>
+        <v>0.16364026743188359</v>
+      </c>
+      <c r="K7" s="70">
+        <f>AVERAGE(C7:G7)</f>
+        <v>0.21409322733653752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="14">
+        <f>income_statement!F19</f>
+        <v>966813</v>
+      </c>
+      <c r="C8" s="68">
+        <f>C9*C2</f>
+        <v>3612623.2846992877</v>
+      </c>
+      <c r="D8" s="68">
+        <f t="shared" ref="D8:G8" si="5">D9*D2</f>
+        <v>3816240.7360662175</v>
+      </c>
+      <c r="E8" s="68">
+        <f t="shared" si="5"/>
+        <v>4031002.0430654702</v>
+      </c>
+      <c r="F8" s="68">
+        <f t="shared" si="5"/>
+        <v>4257491.4308152823</v>
+      </c>
+      <c r="G8" s="68">
+        <f>G9*G2</f>
+        <v>4496321.7122924104</v>
+      </c>
+      <c r="H8" s="66">
+        <f>(highlights!F20/highlights!B20)^(1/4)-1</f>
+        <v>0.25809695791895071</v>
+      </c>
+      <c r="I8" s="66">
+        <f>(G8/B8)^(1/5)-1</f>
+        <v>0.35988749194612102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A9" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="80">
+        <f>B8/B4</f>
+        <v>0.77767160145268521</v>
+      </c>
+      <c r="C9" s="80">
+        <f>B9</f>
+        <v>0.77767160145268521</v>
+      </c>
+      <c r="D9" s="80">
+        <f>C9-0.007</f>
+        <v>0.77067160145268521</v>
+      </c>
+      <c r="E9" s="80">
+        <f t="shared" ref="E9:G9" si="6">D9-0.007</f>
+        <v>0.7636716014526852</v>
+      </c>
+      <c r="F9" s="80">
+        <f t="shared" si="6"/>
+        <v>0.75667160145268519</v>
+      </c>
+      <c r="G9" s="80">
+        <f t="shared" si="6"/>
+        <v>0.74967160145268519</v>
+      </c>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103">
+        <f>highlights!H21</f>
+        <v>0.64542475153627743</v>
+      </c>
+      <c r="K9" s="80">
+        <f>AVERAGE(C9:G9)</f>
+        <v>0.7636716014526852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="57">
+        <v>0</v>
+      </c>
+      <c r="C10" s="57">
+        <v>1</v>
+      </c>
+      <c r="D10" s="57">
+        <v>2</v>
+      </c>
+      <c r="E10" s="57">
+        <v>3</v>
+      </c>
+      <c r="F10" s="57">
+        <v>4</v>
+      </c>
+      <c r="G10" s="57">
+        <v>5</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="J10" s="95" t="s">
+        <v>205</v>
+      </c>
+      <c r="K10" s="95" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B11" s="14">
         <f>ABS(income_statement!F5)</f>
         <v>1620437</v>
       </c>
-      <c r="C3" s="70">
-        <f>B3*(1+$H$3)</f>
-        <v>1745271.5472367122</v>
-      </c>
-      <c r="D3" s="70">
-        <f t="shared" ref="D3:G3" si="0">C3*(1+$H$3)</f>
-        <v>1879723.046063517</v>
-      </c>
-      <c r="E3" s="70">
-        <f t="shared" si="0"/>
-        <v>2024532.3631710333</v>
-      </c>
-      <c r="F3" s="70">
-        <f t="shared" si="0"/>
-        <v>2180497.4398278403</v>
-      </c>
-      <c r="G3" s="70">
-        <f t="shared" si="0"/>
-        <v>2348477.6887679216</v>
-      </c>
-      <c r="H3" s="66">
+      <c r="C11" s="68">
+        <f>C2*C12</f>
+        <v>1743521.6643107254</v>
+      </c>
+      <c r="D11" s="68">
+        <f t="shared" ref="D11:G11" si="7">D2*D12</f>
+        <v>1858520.3397412763</v>
+      </c>
+      <c r="E11" s="68">
+        <f t="shared" si="7"/>
+        <v>1981104.0630788803</v>
+      </c>
+      <c r="F11" s="68">
+        <f t="shared" si="7"/>
+        <v>2111773.1266228775</v>
+      </c>
+      <c r="G11" s="68">
+        <f t="shared" si="7"/>
+        <v>2251060.8208010118</v>
+      </c>
+      <c r="H11" s="66">
         <f>(highlights!F7/highlights!B7)^(1/4)-1</f>
         <v>7.7037581366453667E-2</v>
       </c>
-      <c r="I3" s="62">
-        <f>(G3/B3)^(1/5)-1</f>
-        <v>7.7037581366453667E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="71" t="s">
+      <c r="I11" s="66">
+        <f>(G11/B11)^(1/5)-1</f>
+        <v>6.7950235002587789E-2</v>
+      </c>
+      <c r="J11" s="102"/>
+      <c r="K11" s="64"/>
+    </row>
+    <row r="12" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="72">
-        <f>B3/B2</f>
+      <c r="B12" s="70">
+        <f>B11/B2</f>
         <v>0.37531931175736638</v>
       </c>
-      <c r="C4" s="72">
-        <f t="shared" ref="C4:G4" si="1">C3/C2</f>
-        <v>0.37569600042655876</v>
-      </c>
-      <c r="D4" s="72">
-        <f t="shared" si="1"/>
-        <v>0.37607306715877398</v>
-      </c>
-      <c r="E4" s="72">
-        <f t="shared" si="1"/>
-        <v>0.37645051233345428</v>
-      </c>
-      <c r="F4" s="72">
-        <f t="shared" si="1"/>
-        <v>0.3768283363304229</v>
-      </c>
-      <c r="G4" s="72">
-        <f t="shared" si="1"/>
-        <v>0.37720653952988437</v>
-      </c>
-      <c r="H4" s="80"/>
-      <c r="I4" s="62"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4" t="s">
+      <c r="C12" s="70">
+        <f>B12</f>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="D12" s="70">
+        <f>C12</f>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="E12" s="70">
+        <f t="shared" ref="E12:G12" si="8">D12</f>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="F12" s="70">
+        <f t="shared" si="8"/>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="G12" s="70">
+        <f t="shared" si="8"/>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="H12" s="70"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="102">
+        <f>highlights!H8</f>
+        <v>0.38401157670826447</v>
+      </c>
+      <c r="K12" s="64"/>
+    </row>
+    <row r="13" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B13" s="14">
         <f>ABS(SUM(income_statement!F6:F8))</f>
         <v>1561676</v>
       </c>
-      <c r="C5" s="70">
-        <f>B5*(1+$H$5)</f>
-        <v>1618549.9641978096</v>
-      </c>
-      <c r="D5" s="70">
-        <f t="shared" ref="D5:G5" si="2">C5*(1+$H$5)</f>
-        <v>1677495.1952932174</v>
-      </c>
-      <c r="E5" s="70">
-        <f t="shared" si="2"/>
-        <v>1738587.1258083202</v>
-      </c>
-      <c r="F5" s="70">
-        <f t="shared" si="2"/>
-        <v>1801903.9354077473</v>
-      </c>
-      <c r="G5" s="70">
-        <f t="shared" si="2"/>
-        <v>1867526.6509455875</v>
-      </c>
-      <c r="H5" s="66">
-        <f>(highlights!F8/highlights!B8)^(1/4)-1</f>
+      <c r="C13" s="68">
+        <f>C2*C14</f>
+        <v>1680297.3140172164</v>
+      </c>
+      <c r="D13" s="68">
+        <f t="shared" ref="D13:G13" si="9">D2*D14</f>
+        <v>1791125.8568434301</v>
+      </c>
+      <c r="E13" s="68">
+        <f t="shared" si="9"/>
+        <v>1909264.3952296653</v>
+      </c>
+      <c r="F13" s="68">
+        <f t="shared" si="9"/>
+        <v>2035195.0796556168</v>
+      </c>
+      <c r="G13" s="68">
+        <f t="shared" si="9"/>
+        <v>2169431.8621367207</v>
+      </c>
+      <c r="H13" s="66">
+        <f>(highlights!F9/highlights!B9)^(1/4)-1</f>
         <v>3.6418542769312889E-2</v>
       </c>
-      <c r="I5" s="62">
-        <f t="shared" ref="I5:I14" si="3">(G5/B5)^(1/5)-1</f>
-        <v>3.6418542769312889E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="71" t="s">
+      <c r="I13" s="66">
+        <f>(G13/B13)^(1/5)-1</f>
+        <v>6.7950235002587789E-2</v>
+      </c>
+      <c r="J13" s="102"/>
+      <c r="K13" s="64"/>
+    </row>
+    <row r="14" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="B6" s="72">
-        <f>B5/B2</f>
+      <c r="B14" s="70">
+        <f>B13/B2</f>
         <v>0.36170931761493774</v>
       </c>
-      <c r="C6" s="72">
-        <f t="shared" ref="C6:G6" si="4">C5/C2</f>
-        <v>0.34841727008180712</v>
-      </c>
-      <c r="D6" s="72">
-        <f t="shared" si="4"/>
-        <v>0.33561367700372902</v>
-      </c>
-      <c r="E6" s="72">
-        <f t="shared" si="4"/>
-        <v>0.32328058871914322</v>
-      </c>
-      <c r="F6" s="72">
-        <f t="shared" si="4"/>
-        <v>0.31140071517834661</v>
-      </c>
-      <c r="G6" s="72">
-        <f t="shared" si="4"/>
-        <v>0.29995740170416113</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="62"/>
-    </row>
-    <row r="7" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="14">
-        <f>income_statement!F9</f>
-        <v>1243215</v>
-      </c>
-      <c r="C7" s="70">
-        <f>C2-C3-C5</f>
-        <v>1281614.014243582</v>
-      </c>
-      <c r="D7" s="70">
-        <f t="shared" ref="D7:F7" si="5">D2-D3-D5</f>
-        <v>1441073.8731645062</v>
-      </c>
-      <c r="E7" s="70">
-        <f t="shared" si="5"/>
-        <v>1614831.3886056726</v>
-      </c>
-      <c r="F7" s="70">
-        <f t="shared" si="5"/>
-        <v>1804046.2710896756</v>
-      </c>
-      <c r="G7" s="70">
-        <f>G2-G3-G5</f>
-        <v>2009968.549555189</v>
-      </c>
-      <c r="H7" s="66">
-        <f>(highlights!F9/highlights!B9)^(1/4)-1</f>
-        <v>0.1431104793723732</v>
-      </c>
-      <c r="I7" s="62">
-        <f t="shared" si="3"/>
-        <v>0.10085115927940347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="71" t="s">
+      <c r="C14" s="70">
+        <f>B14</f>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="D14" s="70">
+        <f t="shared" ref="D14:G14" si="10">C14</f>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="E14" s="70">
+        <f t="shared" si="10"/>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="F14" s="70">
+        <f t="shared" si="10"/>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="G14" s="70">
+        <f t="shared" si="10"/>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="102">
+        <f>highlights!H10</f>
+        <v>0.39432857870850252</v>
+      </c>
+      <c r="K14" s="64"/>
+    </row>
+    <row r="15" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="14">
+        <f>B6*(1-highlights!$B$1)</f>
+        <v>787832</v>
+      </c>
+      <c r="C15" s="14">
+        <f>C6*(1-highlights!$B$1)</f>
+        <v>847673.90514857869</v>
+      </c>
+      <c r="D15" s="14">
+        <f>D6*(1-highlights!$B$1)</f>
+        <v>875854.23315416614</v>
+      </c>
+      <c r="E15" s="14">
+        <f>E6*(1-highlights!$B$1)</f>
+        <v>904064.24453486223</v>
+      </c>
+      <c r="F15" s="14">
+        <f>F6*(1-highlights!$B$1)</f>
+        <v>932185.25878066523</v>
+      </c>
+      <c r="G15" s="14">
+        <f>G6*(1-highlights!$B$1)</f>
+        <v>960082.81046000647</v>
+      </c>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+    </row>
+    <row r="16" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="70">
+        <f>B15/B2</f>
+        <v>0.18247458186923002</v>
+      </c>
+      <c r="C16" s="70">
+        <f>C15/C2</f>
+        <v>0.18247458186923002</v>
+      </c>
+      <c r="D16" s="70">
+        <f>D15/D2</f>
+        <v>0.17687458186923</v>
+      </c>
+      <c r="E16" s="70">
+        <f>E15/E2</f>
+        <v>0.17127458186923</v>
+      </c>
+      <c r="F16" s="70">
+        <f>F15/F2</f>
+        <v>0.16567458186923001</v>
+      </c>
+      <c r="G16" s="70">
+        <f>G15/G2</f>
+        <v>0.16007458186922999</v>
+      </c>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+    </row>
+    <row r="17" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B8" s="72">
-        <f>ABS(B7)/$B$2</f>
-        <v>0.28794862013545375</v>
-      </c>
-      <c r="C8" s="72">
-        <f t="shared" ref="C8:G8" si="6">ABS(C7)/$B$2</f>
-        <v>0.29684245037881557</v>
-      </c>
-      <c r="D8" s="72">
-        <f t="shared" si="6"/>
-        <v>0.33377592233923609</v>
-      </c>
-      <c r="E8" s="72">
-        <f t="shared" si="6"/>
-        <v>0.37402096186132094</v>
-      </c>
-      <c r="F8" s="72">
-        <f t="shared" si="6"/>
-        <v>0.4178461765831194</v>
-      </c>
-      <c r="G8" s="72">
-        <f t="shared" si="6"/>
-        <v>0.46554109334272514</v>
-      </c>
-      <c r="H8" s="66"/>
-      <c r="I8" s="62"/>
-    </row>
-    <row r="9" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="B9" s="73" cm="1">
-        <f t="array" ref="B9">SUM(ABS(income_statement!F10:F11))</f>
+      <c r="B17" s="14">
+        <f>ABS(highlights!F13)</f>
         <v>258425</v>
       </c>
-      <c r="C9" s="73">
-        <f>B9*(1+$H$9)</f>
-        <v>258066.00026372526</v>
-      </c>
-      <c r="D9" s="73">
-        <f t="shared" ref="D9:G9" si="7">C9*(1+$H$9)</f>
-        <v>257707.49924394715</v>
-      </c>
-      <c r="E9" s="73">
-        <f t="shared" si="7"/>
-        <v>257349.49624785699</v>
-      </c>
-      <c r="F9" s="73">
-        <f t="shared" si="7"/>
-        <v>256991.99058360848</v>
-      </c>
-      <c r="G9" s="73">
-        <f t="shared" si="7"/>
-        <v>256634.98156031646</v>
-      </c>
-      <c r="H9" s="66">
-        <f>(SUM(income_statement!F10:F11)/SUM(income_statement!B10:B11))^(1/4)-1</f>
+      <c r="C17" s="68">
+        <f>C4*C18</f>
+        <v>278054.36811150273</v>
+      </c>
+      <c r="D17" s="68">
+        <f t="shared" ref="D17:G17" si="11">D4*D18</f>
+        <v>323969.1828007375</v>
+      </c>
+      <c r="E17" s="68">
+        <f t="shared" si="11"/>
+        <v>372883.75839333725</v>
+      </c>
+      <c r="F17" s="68">
+        <f t="shared" si="11"/>
+        <v>424872.20686973305</v>
+      </c>
+      <c r="G17" s="68">
+        <f t="shared" si="11"/>
+        <v>479997.32929640211</v>
+      </c>
+      <c r="H17" s="66">
+        <f>highlights!G13</f>
         <v>-1.3891834624155663E-3</v>
       </c>
-      <c r="I9" s="62"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="14">
-        <f>income_statement!F12</f>
-        <v>984790</v>
-      </c>
-      <c r="C10" s="70">
-        <f>C7-C9</f>
-        <v>1023548.0139798567</v>
-      </c>
-      <c r="D10" s="70">
-        <f t="shared" ref="D10:G10" si="8">D7-D9</f>
-        <v>1183366.373920559</v>
-      </c>
-      <c r="E10" s="70">
-        <f t="shared" si="8"/>
-        <v>1357481.8923578155</v>
-      </c>
-      <c r="F10" s="70">
-        <f t="shared" si="8"/>
-        <v>1547054.2805060672</v>
-      </c>
-      <c r="G10" s="70">
-        <f t="shared" si="8"/>
-        <v>1753333.5679948726</v>
-      </c>
-      <c r="H10" s="66">
-        <f>(highlights!F10/highlights!B10)^(1/4)-1</f>
-        <v>0.20425717756209383</v>
-      </c>
-      <c r="I10" s="62">
-        <f t="shared" si="3"/>
-        <v>0.12228764920764212</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="72">
-        <f>ABS(B10)/$B$2</f>
-        <v>0.2280932273365375</v>
-      </c>
-      <c r="C11" s="72">
-        <f>ABS(C10)/$B$2</f>
-        <v>0.23707020770171197</v>
-      </c>
-      <c r="D11" s="72">
-        <f t="shared" ref="D11:G11" si="9">ABS(D10)/$B$2</f>
-        <v>0.27408671427317105</v>
-      </c>
-      <c r="E11" s="72">
-        <f t="shared" si="9"/>
-        <v>0.31441467305598592</v>
-      </c>
-      <c r="F11" s="72">
-        <f t="shared" si="9"/>
-        <v>0.35832269184844878</v>
-      </c>
-      <c r="G11" s="72">
-        <f t="shared" si="9"/>
-        <v>0.40610029764867323</v>
-      </c>
-      <c r="H11" s="66"/>
-      <c r="I11" s="62"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="4" t="s">
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+    </row>
+    <row r="18" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="70">
+        <f>ABS(B17)/B4</f>
+        <v>0.2078683091822412</v>
+      </c>
+      <c r="C18" s="70">
+        <f>B18</f>
+        <v>0.2078683091822412</v>
+      </c>
+      <c r="D18" s="70">
+        <f>C18+0.025</f>
+        <v>0.23286830918224119</v>
+      </c>
+      <c r="E18" s="70">
+        <f t="shared" ref="E18:G18" si="12">D18+0.025</f>
+        <v>0.25786830918224118</v>
+      </c>
+      <c r="F18" s="70">
+        <f t="shared" si="12"/>
+        <v>0.28286830918224121</v>
+      </c>
+      <c r="G18" s="70">
+        <f t="shared" si="12"/>
+        <v>0.30786830918224123</v>
+      </c>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="66">
+        <f>highlights!H14</f>
+        <v>0.32946259858537613</v>
+      </c>
+      <c r="K18" s="102">
+        <f>AVERAGE(B18:G18)</f>
+        <v>0.24953497584890785</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B19" s="14">
         <f>SUM(income_statement!F13:F16)</f>
         <v>156079</v>
       </c>
-      <c r="C12" s="70">
-        <f>B12*(1+$H$12)</f>
+      <c r="C19" s="68">
+        <f>B19*(1+$H$19)</f>
         <v>162719.02739330876</v>
       </c>
-      <c r="D12" s="70">
-        <f t="shared" ref="D12:G12" si="10">C12*(1+$H$12)</f>
+      <c r="D19" s="68">
+        <f>C19*(1+$H$19)</f>
         <v>169641.53970633054</v>
       </c>
-      <c r="E12" s="70">
-        <f t="shared" si="10"/>
+      <c r="E19" s="68">
+        <f>D19*(1+$H$19)</f>
         <v>176858.55461988784</v>
       </c>
-      <c r="F12" s="70">
-        <f t="shared" si="10"/>
+      <c r="F19" s="68">
+        <f>E19*(1+$H$19)</f>
         <v>184382.60107980267</v>
       </c>
-      <c r="G12" s="70">
-        <f t="shared" si="10"/>
+      <c r="G19" s="68">
+        <f>F19*(1+$H$19)</f>
         <v>192226.74104750756</v>
       </c>
-      <c r="H12" s="66">
-        <f>(ABS(highlights!F15)/ABS(highlights!B15))^(1/4)-1</f>
+      <c r="H19" s="66">
+        <f>(ABS(highlights!F23)/ABS(highlights!B23))^(1/4)-1</f>
         <v>4.2542734085359024E-2</v>
       </c>
-      <c r="I12" s="62"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="72">
-        <f>B12/B2</f>
-        <v>3.615041057429446E-2</v>
-      </c>
-      <c r="C13" s="72">
-        <f>C12/C2</f>
-        <v>3.5027722695506858E-2</v>
-      </c>
-      <c r="D13" s="72">
-        <f>D12/D2</f>
-        <v>3.3939901034091439E-2</v>
-      </c>
-      <c r="E13" s="72">
-        <f>E12/E2</f>
-        <v>3.288586278409935E-2</v>
-      </c>
-      <c r="F13" s="72">
-        <f>F12/F2</f>
-        <v>3.186455876722509E-2</v>
-      </c>
-      <c r="G13" s="72">
-        <f>G12/G2</f>
-        <v>3.0874972388465777E-2</v>
-      </c>
-      <c r="H13" s="66"/>
-      <c r="I13" s="62"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="14">
-        <f>income_statement!F19</f>
-        <v>966813</v>
-      </c>
-      <c r="C14" s="70">
-        <f>(C10+C12)*(1-highlights!$B$1)</f>
-        <v>949013.63309853245</v>
-      </c>
-      <c r="D14" s="70">
-        <f>(D10+D12)*(1-highlights!$B$1)</f>
-        <v>1082406.3309015117</v>
-      </c>
-      <c r="E14" s="70">
-        <f>(E10+E12)*(1-highlights!$B$1)</f>
-        <v>1227472.3575821628</v>
-      </c>
-      <c r="F14" s="70">
-        <f>(F10+F12)*(1-highlights!$B$1)</f>
-        <v>1385149.505268696</v>
-      </c>
-      <c r="G14" s="70">
-        <f>(G10+G12)*(1-highlights!$B$1)</f>
-        <v>1556448.2472339042</v>
-      </c>
-      <c r="H14" s="66">
-        <f>(highlights!F12/highlights!B12)^(1/4)-1</f>
-        <v>0.25809695791895071</v>
-      </c>
-      <c r="I14" s="62">
-        <f t="shared" si="3"/>
-        <v>9.9913267473285883E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="102" customFormat="1" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="84" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="85">
-        <f>ABS(B14)/$B$2</f>
-        <v>0.22392946455682922</v>
-      </c>
-      <c r="C15" s="85">
-        <f t="shared" ref="C15" si="11">ABS(C14)/$B$2</f>
-        <v>0.21980684446411616</v>
-      </c>
-      <c r="D15" s="85">
-        <f t="shared" ref="D15" si="12">ABS(D14)/$B$2</f>
-        <v>0.25070274201081039</v>
-      </c>
-      <c r="E15" s="85">
-        <f t="shared" ref="E15" si="13">ABS(E14)/$B$2</f>
-        <v>0.28430237056357593</v>
-      </c>
-      <c r="F15" s="85">
-        <f t="shared" ref="F15" si="14">ABS(F14)/$B$2</f>
-        <v>0.32082293788558486</v>
-      </c>
-      <c r="G15" s="85">
-        <f t="shared" ref="G15" si="15">ABS(G14)/$B$2</f>
-        <v>0.36049848586386768</v>
-      </c>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87"/>
-    </row>
-    <row r="16" spans="1:9" s="102" customFormat="1" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="57">
-        <v>0</v>
-      </c>
-      <c r="C16" s="57">
-        <v>1</v>
-      </c>
-      <c r="D16" s="57">
-        <v>2</v>
-      </c>
-      <c r="E16" s="57">
-        <v>3</v>
-      </c>
-      <c r="F16" s="57">
-        <v>4</v>
-      </c>
-      <c r="G16" s="57">
-        <v>5</v>
-      </c>
-      <c r="H16" s="69" t="s">
-        <v>164</v>
-      </c>
-      <c r="I16" s="103" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="102" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="14">
-        <f>B10*(1-highlights!$B$1)</f>
-        <v>787832</v>
-      </c>
-      <c r="C17" s="14">
-        <f>C10*(1-highlights!$B$1)</f>
-        <v>818838.41118388542</v>
-      </c>
-      <c r="D17" s="14">
-        <f>D10*(1-highlights!$B$1)</f>
-        <v>946693.09913644718</v>
-      </c>
-      <c r="E17" s="14">
-        <f>E10*(1-highlights!$B$1)</f>
-        <v>1085985.5138862524</v>
-      </c>
-      <c r="F17" s="14">
-        <f>F10*(1-highlights!$B$1)</f>
-        <v>1237643.4244048537</v>
-      </c>
-      <c r="G17" s="14">
-        <f>G10*(1-highlights!$B$1)</f>
-        <v>1402666.8543958981</v>
-      </c>
-      <c r="H17" s="68"/>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="72">
-        <f>B17/B2</f>
-        <v>0.18247458186923002</v>
-      </c>
-      <c r="C18" s="72">
-        <f>C17/C2</f>
-        <v>0.17626730726487866</v>
-      </c>
-      <c r="D18" s="72">
-        <f>D17/D2</f>
-        <v>0.18940331566177895</v>
-      </c>
-      <c r="E18" s="72">
-        <f>E17/E2</f>
-        <v>0.20193295524742969</v>
-      </c>
-      <c r="F18" s="72">
-        <f>F17/F2</f>
-        <v>0.21388656738142797</v>
-      </c>
-      <c r="G18" s="72">
-        <f>G17/G2</f>
-        <v>0.22529279830523885</v>
-      </c>
-      <c r="H18" s="68"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" s="76">
-        <f>ABS(highlights!F15)</f>
-        <v>303704</v>
-      </c>
-      <c r="C19" s="77">
-        <f>B19*(1+$H$19)</f>
-        <v>316624.39851265989</v>
-      </c>
-      <c r="D19" s="77">
-        <f t="shared" ref="D19:G19" si="16">C19*(1+$H$19)</f>
-        <v>330094.46610352071</v>
-      </c>
-      <c r="E19" s="77">
-        <f t="shared" si="16"/>
-        <v>344137.58719801134</v>
-      </c>
-      <c r="F19" s="77">
-        <f t="shared" si="16"/>
-        <v>358778.14105895342</v>
-      </c>
-      <c r="G19" s="77">
-        <f t="shared" si="16"/>
-        <v>374041.54410966393</v>
-      </c>
-      <c r="H19" s="62">
-        <f>highlights!G15</f>
-        <v>4.2542734085359024E-2</v>
-      </c>
-      <c r="I19" s="62">
+      <c r="I19" s="66">
         <f>(G19/B19)^(1/5)-1</f>
         <v>4.2542734085359024E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="71" t="s">
+      <c r="J19" s="102"/>
+      <c r="K19" s="64"/>
+    </row>
+    <row r="20" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="72">
+      <c r="B20" s="70">
         <f>B19/B2</f>
-        <v>7.0342738568644883E-2</v>
-      </c>
-      <c r="C20" s="72">
+        <v>3.615041057429446E-2</v>
+      </c>
+      <c r="C20" s="70">
         <f>C19/C2</f>
-        <v>6.8158173063104038E-2</v>
-      </c>
-      <c r="D20" s="72">
+        <v>3.5027722695506858E-2</v>
+      </c>
+      <c r="D20" s="70">
         <f>D19/D2</f>
-        <v>6.6041451467895779E-2</v>
-      </c>
-      <c r="E20" s="72">
+        <v>3.4258299232228659E-2</v>
+      </c>
+      <c r="E20" s="70">
         <f>E19/E2</f>
-        <v>6.3990466821174583E-2</v>
-      </c>
-      <c r="F20" s="72">
+        <v>3.3505777023736263E-2</v>
+      </c>
+      <c r="F20" s="70">
         <f>F19/F2</f>
-        <v>6.200317759494442E-2</v>
-      </c>
-      <c r="G20" s="72">
+        <v>3.2769784814892573E-2</v>
+      </c>
+      <c r="G20" s="70">
         <f>G19/G2</f>
-        <v>6.0077605662943831E-2</v>
-      </c>
-      <c r="H20" s="68"/>
-    </row>
-    <row r="21" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>3.2049959505598621E-2</v>
+      </c>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="64"/>
+    </row>
+    <row r="21" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B21" s="14">
-        <f>highlights!F35</f>
-        <v>1014099</v>
-      </c>
-      <c r="C21" s="70">
-        <f>B21*(1+$H$21)</f>
-        <v>1198499.406907514</v>
-      </c>
-      <c r="D21" s="70">
-        <f t="shared" ref="D21:F21" si="17">C21*(1+$H$21)</f>
-        <v>1416430.5736990795</v>
-      </c>
-      <c r="E21" s="70">
-        <f t="shared" si="17"/>
-        <v>1673989.6228119903</v>
-      </c>
-      <c r="F21" s="70">
-        <f t="shared" si="17"/>
-        <v>1978382.3572545713</v>
-      </c>
-      <c r="G21" s="70">
-        <f>F21*(1+$H$21)</f>
-        <v>2338124.8594130292</v>
+        <v>150</v>
+      </c>
+      <c r="B21" s="73">
+        <f>ABS(highlights!F23)</f>
+        <v>303704</v>
+      </c>
+      <c r="C21" s="74">
+        <f>C22*C2</f>
+        <v>303545.47909187974</v>
+      </c>
+      <c r="D21" s="74">
+        <f t="shared" ref="D21:G21" si="13">D22*D2</f>
+        <v>298807.45134163956</v>
+      </c>
+      <c r="E21" s="74">
+        <f t="shared" si="13"/>
+        <v>292123.8550899126</v>
+      </c>
+      <c r="F21" s="74">
+        <f t="shared" si="13"/>
+        <v>283258.65229816205</v>
+      </c>
+      <c r="G21" s="74">
+        <f t="shared" si="13"/>
+        <v>271953.13191260578</v>
       </c>
       <c r="H21" s="66">
-        <f>highlights!G35</f>
-        <v>0.18183669139552849</v>
+        <f>highlights!G23</f>
+        <v>4.2542734085359024E-2</v>
       </c>
       <c r="I21" s="66">
         <f>(G21/B21)^(1/5)-1</f>
+        <v>-2.1842677185442416E-2</v>
+      </c>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+    </row>
+    <row r="22" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="70">
+        <f>B21/B2</f>
+        <v>7.0342738568644883E-2</v>
+      </c>
+      <c r="C22" s="70">
+        <f>B22-0.005</f>
+        <v>6.5342738568644879E-2</v>
+      </c>
+      <c r="D22" s="70">
+        <f t="shared" ref="D22:G22" si="14">C22-0.005</f>
+        <v>6.0342738568644881E-2</v>
+      </c>
+      <c r="E22" s="70">
+        <f t="shared" si="14"/>
+        <v>5.5342738568644884E-2</v>
+      </c>
+      <c r="F22" s="70">
+        <f t="shared" si="14"/>
+        <v>5.0342738568644886E-2</v>
+      </c>
+      <c r="G22" s="70">
+        <f t="shared" si="14"/>
+        <v>4.5342738568644889E-2</v>
+      </c>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+    </row>
+    <row r="23" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23" s="14">
+        <f>highlights!F43</f>
+        <v>1014099</v>
+      </c>
+      <c r="C23" s="68">
+        <f>C24*C2</f>
+        <v>1067900.4479786786</v>
+      </c>
+      <c r="D23" s="68">
+        <f t="shared" ref="D23:G23" si="15">D24*D2</f>
+        <v>1113577.5144483843</v>
+      </c>
+      <c r="E23" s="68">
+        <f t="shared" si="15"/>
+        <v>1160634.2759769456</v>
+      </c>
+      <c r="F23" s="68">
+        <f t="shared" si="15"/>
+        <v>1209054.0212555847</v>
+      </c>
+      <c r="G23" s="68">
+        <f t="shared" si="15"/>
+        <v>1258811.8322464877</v>
+      </c>
+      <c r="H23" s="66">
+        <f>highlights!G43</f>
         <v>0.18183669139552849</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="71" t="s">
+      <c r="I23" s="66">
+        <f>(G23/B23)^(1/5)-1</f>
+        <v>4.4181735488849849E-2</v>
+      </c>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+    </row>
+    <row r="24" spans="1:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="B22" s="78">
-        <f>B21/B2</f>
+      <c r="B24" s="75">
+        <f>B23/B2</f>
         <v>0.2348816638560052</v>
       </c>
-      <c r="C22" s="78">
-        <f>C21/C2</f>
-        <v>0.25799505779010173</v>
-      </c>
-      <c r="D22" s="78">
-        <f>D21/D2</f>
-        <v>0.28338291185183195</v>
-      </c>
-      <c r="E22" s="78">
-        <f>E21/E2</f>
-        <v>0.31126904297119518</v>
-      </c>
-      <c r="F22" s="78">
-        <f>F21/F2</f>
-        <v>0.34189929265340563</v>
-      </c>
-      <c r="G22" s="78">
-        <f>G21/G2</f>
-        <v>0.37554369429444545</v>
-      </c>
-      <c r="H22" s="66"/>
-    </row>
-    <row r="23" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="4" t="s">
+      <c r="C24" s="75">
+        <f>B24-0.005</f>
+        <v>0.2298816638560052</v>
+      </c>
+      <c r="D24" s="75">
+        <f t="shared" ref="D24:G24" si="16">C24-0.005</f>
+        <v>0.22488166385600519</v>
+      </c>
+      <c r="E24" s="75">
+        <f t="shared" si="16"/>
+        <v>0.21988166385600519</v>
+      </c>
+      <c r="F24" s="75">
+        <f t="shared" si="16"/>
+        <v>0.21488166385600518</v>
+      </c>
+      <c r="G24" s="75">
+        <f t="shared" si="16"/>
+        <v>0.20988166385600518</v>
+      </c>
+      <c r="H24" s="66"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="66">
+        <f>highlights!H44</f>
+        <v>0.16938979430298501</v>
+      </c>
+      <c r="K24" s="64"/>
+    </row>
+    <row r="25" spans="1:11" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="14">
-        <f>highlights!F37</f>
+      <c r="B25" s="104">
+        <f>highlights!F45</f>
         <v>214468</v>
       </c>
-      <c r="C23" s="14">
-        <f>C21-B21</f>
-        <v>184400.40690751397</v>
-      </c>
-      <c r="D23" s="14">
-        <f t="shared" ref="D23:G23" si="18">D21-C21</f>
-        <v>217931.16679156548</v>
-      </c>
-      <c r="E23" s="14">
+      <c r="C25" s="104">
+        <f>C23-B23</f>
+        <v>53801.447978678625</v>
+      </c>
+      <c r="D25" s="104">
+        <f t="shared" ref="D25:G25" si="17">D23-C23</f>
+        <v>45677.066469705664</v>
+      </c>
+      <c r="E25" s="104">
+        <f t="shared" si="17"/>
+        <v>47056.761528561357</v>
+      </c>
+      <c r="F25" s="104">
+        <f t="shared" si="17"/>
+        <v>48419.74527863902</v>
+      </c>
+      <c r="G25" s="104">
+        <f t="shared" si="17"/>
+        <v>49757.810990903061</v>
+      </c>
+      <c r="H25" s="12">
+        <f>AVERAGE(highlights!D45:F45)</f>
+        <v>226619.66666666666</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="14">
+        <f>B15+B17-B21-B25</f>
+        <v>528085</v>
+      </c>
+      <c r="C26" s="14">
+        <f t="shared" ref="C26:G26" si="18">C15+C17-C21-C25</f>
+        <v>768381.34618952312</v>
+      </c>
+      <c r="D26" s="14">
         <f t="shared" si="18"/>
-        <v>257559.04911291087</v>
-      </c>
-      <c r="F23" s="14">
+        <v>855338.89814355853</v>
+      </c>
+      <c r="E26" s="14">
         <f t="shared" si="18"/>
-        <v>304392.73444258096</v>
-      </c>
-      <c r="G23" s="14">
+        <v>937767.38630972547</v>
+      </c>
+      <c r="F26" s="14">
         <f t="shared" si="18"/>
-        <v>359742.50215845788</v>
-      </c>
-      <c r="H23" s="81">
-        <f>AVERAGE(highlights!D37:F37)</f>
-        <v>226619.66666666666</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="4" t="s">
+        <v>1025379.0680735973</v>
+      </c>
+      <c r="G26" s="14">
+        <f t="shared" si="18"/>
+        <v>1118369.1968528996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A27" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" s="105">
+        <f>B26/B2</f>
+        <v>0.12231299257508242</v>
+      </c>
+      <c r="C27" s="105">
+        <f>C26/C2</f>
+        <v>0.1654056636761439</v>
+      </c>
+      <c r="D27" s="105">
+        <f>D26/D2</f>
+        <v>0.17273160788503086</v>
+      </c>
+      <c r="E27" s="105">
+        <f>E26/E2</f>
+        <v>0.17765962756710404</v>
+      </c>
+      <c r="F27" s="105">
+        <f>F26/F2</f>
+        <v>0.18223764724917732</v>
+      </c>
+      <c r="G27" s="105">
+        <f>G26/G2</f>
+        <v>0.1864656669312505</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" s="11">
+        <f>C26/(1+assumptions!$B$5)^C10</f>
+        <v>698528.49653593008</v>
+      </c>
+      <c r="D28" s="11">
+        <f>D26/(1+assumptions!$B$5)^D10</f>
+        <v>706891.65135831269</v>
+      </c>
+      <c r="E28" s="11">
+        <f>E26/(1+assumptions!$B$5)^E10</f>
+        <v>704558.51713728416</v>
+      </c>
+      <c r="F28" s="11">
+        <f>F26/(1+assumptions!$B$5)^F10</f>
+        <v>700347.70034396357</v>
+      </c>
+      <c r="G28" s="11">
+        <f>G26/(1+assumptions!$B$5)^G10</f>
+        <v>694419.28137850692</v>
+      </c>
+      <c r="H28" s="56"/>
+    </row>
+    <row r="29" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="62">
+        <f>B26/B4</f>
+        <v>0.42477367148884143</v>
+      </c>
+      <c r="C29" s="62">
+        <f>C26/C4</f>
+        <v>0.5744277003249243</v>
+      </c>
+      <c r="D29" s="62">
+        <f>D26/D4</f>
+        <v>0.61481564779265252</v>
+      </c>
+      <c r="E29" s="62">
+        <f>E26/E4</f>
+        <v>0.64851440930514759</v>
+      </c>
+      <c r="F29" s="62">
+        <f>F26/F4</f>
+        <v>0.6826693734423771</v>
+      </c>
+      <c r="G29" s="62">
+        <f>G26/G4</f>
+        <v>0.71731739462239574</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="62">
+        <f>B26/B6</f>
+        <v>0.53624122909452776</v>
+      </c>
+      <c r="C30" s="62">
+        <f>C26/C6</f>
+        <v>0.72516692234836955</v>
+      </c>
+      <c r="D30" s="62">
+        <f>D26/D6</f>
+        <v>0.78126141612699473</v>
+      </c>
+      <c r="E30" s="62">
+        <f>E26/E6</f>
+        <v>0.82982366970365329</v>
+      </c>
+      <c r="F30" s="62">
+        <f>F26/F6</f>
+        <v>0.87997878826346887</v>
+      </c>
+      <c r="G30" s="62">
+        <f>G26/G6</f>
+        <v>0.93189394470425158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="76" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="77">
+        <f>highlights!F32</f>
+        <v>5120204</v>
+      </c>
+      <c r="C31" s="77">
+        <f>B31*(1+$H$31)</f>
+        <v>5403095.9493718129</v>
+      </c>
+      <c r="D31" s="77">
+        <f>C31*(1+$H$31)</f>
+        <v>5701617.7164265513</v>
+      </c>
+      <c r="E31" s="77">
+        <f>D31*(1+$H$31)</f>
+        <v>6016632.8506619781</v>
+      </c>
+      <c r="F31" s="77">
+        <f>E31*(1+$H$31)</f>
+        <v>6349052.6128000207</v>
+      </c>
+      <c r="G31" s="77">
+        <f>F31*(1+$H$31)</f>
+        <v>6699838.6108382242</v>
+      </c>
+      <c r="H31" s="62">
+        <f>(highlights!F32/highlights!B32)^(1/4)-1</f>
+        <v>5.5250132489215842E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A32" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B25" s="14">
-        <f>B17+B9-B19-B23</f>
-        <v>528085</v>
-      </c>
-      <c r="C25" s="14">
-        <f t="shared" ref="C25:G25" si="19">C17+C9-C19-C23</f>
-        <v>575879.60602743691</v>
-      </c>
-      <c r="D25" s="14">
+      <c r="B32" s="82">
+        <f>B15/B31</f>
+        <v>0.15386730684949271</v>
+      </c>
+      <c r="C32" s="82">
+        <f t="shared" ref="C32:G32" si="19">C15/C31</f>
+        <v>0.15688670219656806</v>
+      </c>
+      <c r="D32" s="82">
         <f t="shared" si="19"/>
-        <v>656374.96548530809</v>
-      </c>
-      <c r="E25" s="14">
+        <v>0.15361503992644066</v>
+      </c>
+      <c r="E32" s="82">
         <f t="shared" si="19"/>
-        <v>741638.37382318708</v>
-      </c>
-      <c r="F25" s="14">
+        <v>0.15026082976550462</v>
+      </c>
+      <c r="F32" s="82">
         <f t="shared" si="19"/>
-        <v>831464.53948692768</v>
-      </c>
-      <c r="G25" s="14">
+        <v>0.14682273334785906</v>
+      </c>
+      <c r="G32" s="82">
         <f t="shared" si="19"/>
-        <v>925517.78968809266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="71" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="78">
-        <f>B25/B2</f>
-        <v>0.12231299257508242</v>
-      </c>
-      <c r="C26" s="78">
-        <f>C25/C2</f>
-        <v>0.12396676325485641</v>
-      </c>
-      <c r="D26" s="78">
-        <f>D25/D2</f>
-        <v>0.13131984894968041</v>
-      </c>
-      <c r="E26" s="78">
-        <f>E25/E2</f>
-        <v>0.13790352323861693</v>
-      </c>
-      <c r="F26" s="78">
-        <f>F25/F2</f>
-        <v>0.14369170695166608</v>
-      </c>
-      <c r="G26" s="78">
-        <f>G25/G2</f>
-        <v>0.14865432377377472</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C27" s="11">
-        <f>C25/(1+assumptions!$B$5)^C16</f>
-        <v>523526.91457039717</v>
-      </c>
-      <c r="D27" s="11">
-        <f>D25/(1+assumptions!$B$5)^D16</f>
-        <v>542458.64916141157</v>
-      </c>
-      <c r="E27" s="11">
-        <f>E25/(1+assumptions!$B$5)^E16</f>
-        <v>557203.88716993749</v>
-      </c>
-      <c r="F27" s="11">
-        <f>F25/(1+assumptions!$B$5)^F16</f>
-        <v>567901.46812849364</v>
-      </c>
-      <c r="G27" s="11">
-        <f>G25/(1+assumptions!$B$5)^G16</f>
-        <v>574673.73048791522</v>
-      </c>
-      <c r="H27" s="56"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="62">
-        <f>B25/B7</f>
-        <v>0.42477367148884143</v>
-      </c>
-      <c r="C28" s="62">
-        <f>C25/C7</f>
-        <v>0.44933934837418682</v>
-      </c>
-      <c r="D28" s="62">
-        <f>D25/D7</f>
-        <v>0.45547627898072329</v>
-      </c>
-      <c r="E28" s="62">
-        <f>E25/E7</f>
-        <v>0.45926675630423264</v>
-      </c>
-      <c r="F28" s="62">
-        <f>F25/F7</f>
-        <v>0.46088869937061455</v>
-      </c>
-      <c r="G28" s="62">
-        <f>G25/G7</f>
-        <v>0.46046381665668951</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
-        <v>172</v>
-      </c>
-      <c r="B29" s="62">
-        <f>B25/B10</f>
-        <v>0.53624122909452776</v>
-      </c>
-      <c r="C29" s="62">
-        <f>C25/C10</f>
-        <v>0.56263076881781737</v>
-      </c>
-      <c r="D29" s="62">
-        <f>D25/D10</f>
-        <v>0.55466758220507917</v>
-      </c>
-      <c r="E29" s="62">
-        <f>E25/E10</f>
-        <v>0.54633389807876742</v>
-      </c>
-      <c r="F29" s="62">
-        <f>F25/F10</f>
-        <v>0.5374501398974455</v>
-      </c>
-      <c r="G29" s="62">
-        <f>G25/G10</f>
-        <v>0.52786178658891636</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="79" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="82">
-        <f>highlights!F24</f>
-        <v>5120204</v>
-      </c>
-      <c r="C30" s="82">
-        <f>B30*(1+$H$30)</f>
-        <v>5403095.9493718129</v>
-      </c>
-      <c r="D30" s="82">
-        <f>C30*(1+$H$30)</f>
-        <v>5701617.7164265513</v>
-      </c>
-      <c r="E30" s="82">
-        <f>D30*(1+$H$30)</f>
-        <v>6016632.8506619781</v>
-      </c>
-      <c r="F30" s="82">
-        <f>E30*(1+$H$30)</f>
-        <v>6349052.6128000207</v>
-      </c>
-      <c r="G30" s="82">
-        <f>F30*(1+$H$30)</f>
-        <v>6699838.6108382242</v>
-      </c>
-      <c r="H30" s="62">
-        <f>(highlights!F24/highlights!B24)^(1/4)-1</f>
-        <v>5.5250132489215842E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A31" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="89">
-        <f>B17/highlights!F24</f>
-        <v>0.15386730684949271</v>
-      </c>
-      <c r="C31" s="89">
-        <f>B17/C30</f>
-        <v>0.14581121775037081</v>
-      </c>
-      <c r="D31" s="89">
-        <f>C17/D30</f>
-        <v>0.14361510222349433</v>
-      </c>
-      <c r="E31" s="89">
-        <f>D17/E30</f>
-        <v>0.15734599777553113</v>
-      </c>
-      <c r="F31" s="89">
-        <f>E17/F30</f>
-        <v>0.17104686007749392</v>
-      </c>
-      <c r="G31" s="89">
-        <f>F17/G30</f>
-        <v>0.18472734886520062</v>
-      </c>
-      <c r="H31" s="90">
-        <f>AVERAGE(highlights!B42:F42)</f>
+        <v>0.14329939364612387</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="83">
+        <f>AVERAGE(highlights!B50:F50)</f>
         <v>0.10889795982966539</v>
       </c>
-      <c r="I31" s="91">
-        <f>AVERAGE(B31:G31)</f>
-        <v>0.15940230559026392</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>190</v>
-      </c>
-      <c r="B33" s="83">
-        <v>3.8199999999999998E-2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>196</v>
+      <c r="K32" s="84">
+        <f>AVERAGE(B32:G32)</f>
+        <v>0.15079200095533149</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>191</v>
-      </c>
-      <c r="B34" s="50">
-        <v>0.12</v>
+        <v>188</v>
+      </c>
+      <c r="B34" s="78">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B35" s="62">
-        <f ca="1">B33+assumptions!F2*(dcf!B34-dcf!B33)</f>
-        <v>0.11716972</v>
+        <v>189</v>
+      </c>
+      <c r="B35" s="50">
+        <v>0.12</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B36" s="62">
-        <f>ABS(income_statement!F16)/highlights!F20</f>
-        <v>0.16996393425391862</v>
+        <f ca="1">B34+assumptions!F2*(dcf!B35-dcf!B34)</f>
+        <v>0.1167822</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="56">
-        <f>highlights!F26</f>
-        <v>966545</v>
+        <v>191</v>
+      </c>
+      <c r="B37" s="62">
+        <f>ABS(income_statement!F16)/highlights!F28</f>
+        <v>0.16996393425391862</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>136</v>
-      </c>
-      <c r="B38" s="11">
-        <f>highlights!F22</f>
-        <v>-511824</v>
+        <v>99</v>
+      </c>
+      <c r="B38" s="56">
+        <f>highlights!F34</f>
+        <v>966545</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" s="104">
-        <f>B37/(B37+B38)</f>
-        <v>2.1255781017371089</v>
+        <v>136</v>
+      </c>
+      <c r="B39" s="11">
+        <f>IF(highlights!F30&lt;0,highlights!F28,highlights!F30)</f>
+        <v>608888</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B40" s="105">
-        <f>B38/(B37+B38)</f>
-        <v>-1.1255781017371091</v>
+      <c r="A40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="96">
+        <f>B38/(B38+B39)</f>
+        <v>0.61351069832865002</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="97">
+        <f>B39/(B38+B39)</f>
+        <v>0.38648930167135004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B41" s="65">
-        <f ca="1">B39*B35+B40*B36*(1-highlights!B1)</f>
-        <v>9.6007245033631339E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="B43" s="81">
-        <f>(G25*(1+0.02))/(assumptions!B5-assumptions!B4)</f>
-        <v>11800351.818523182</v>
+      <c r="B42" s="65">
+        <f ca="1">B40*B36+B41*B37*(1-highlights!B1)</f>
+        <v>0.12419852288164587</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B44" s="81">
-        <f>B43/(1+0.1)^5</f>
-        <v>7327090.0637209192</v>
+        <v>173</v>
+      </c>
+      <c r="B44" s="11">
+        <f ca="1">(G26*(1+0.02))/(B42-assumptions!B4)</f>
+        <v>15374114.422864558</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B45" s="81">
-        <f>SUM(C27:G27,B44)</f>
-        <v>10092854.713239074</v>
+        <v>176</v>
+      </c>
+      <c r="B45" s="11">
+        <f ca="1">B44/(1+B42)^5</f>
+        <v>8561996.7251677532</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B46" s="81">
-        <f>B45-highlights!F22</f>
-        <v>10604678.713239074</v>
+        <v>177</v>
+      </c>
+      <c r="B46" s="11">
+        <f ca="1">SUM(C28:G28,B45)</f>
+        <v>12066742.371921752</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" s="88">
-        <f>B46/highlights!F28 * 1000</f>
-        <v>57.281766484914783</v>
+        <v>179</v>
+      </c>
+      <c r="B47" s="11">
+        <f ca="1">B46-highlights!F30</f>
+        <v>12578566.371921752</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B48" s="75">
-        <f ca="1">assumptions!D2</f>
-        <v>50.6</v>
+        <v>180</v>
+      </c>
+      <c r="B48" s="81">
+        <f ca="1">B47/highlights!F36 * 1000</f>
+        <v>67.943831313994465</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B49" s="62">
-        <f ca="1">B47/B48-1</f>
-        <v>0.13205072104574667</v>
+        <v>185</v>
+      </c>
+      <c r="B49" s="72">
+        <f ca="1">assumptions!D2</f>
+        <v>45.78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="62">
+        <f ca="1">B48/B49-1</f>
+        <v>0.48413786181726648</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B49">
+  <conditionalFormatting sqref="B50">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -3180,10 +3405,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A1E1FA-E967-47B0-B93E-C43E58801B3E}">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3239,10 +3464,10 @@
         <v>2023</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="I5" s="57" t="s">
         <v>131</v>
@@ -3331,7 +3556,7 @@
         <v>1620437</v>
       </c>
       <c r="G7" s="62">
-        <f t="shared" ref="G7:G38" si="1">(F7/B7)^(1/4)-1</f>
+        <f t="shared" ref="G7:G46" si="1">(F7/B7)^(1/4)-1</f>
         <v>7.7037581366453667E-2</v>
       </c>
       <c r="H7" s="63"/>
@@ -3341,34 +3566,34 @@
       <c r="L7" s="63"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="11">
-        <f>ABS(SUM(income_statement!B6:B8))</f>
-        <v>1353475</v>
-      </c>
-      <c r="C8" s="11">
-        <f>ABS(SUM(income_statement!C6:C8))</f>
-        <v>1317980</v>
-      </c>
-      <c r="D8" s="11">
-        <f>ABS(SUM(income_statement!D6:D8))</f>
-        <v>1368440</v>
-      </c>
-      <c r="E8" s="11">
-        <f>ABS(SUM(income_statement!E6:E8))</f>
-        <v>1532770</v>
-      </c>
-      <c r="F8" s="11">
-        <f>ABS(SUM(income_statement!F6:F8))</f>
-        <v>1561676</v>
-      </c>
-      <c r="G8" s="62">
-        <f t="shared" si="1"/>
-        <v>3.6418542769312889E-2</v>
-      </c>
-      <c r="H8" s="63"/>
+      <c r="A8" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="101">
+        <f>B7/B6</f>
+        <v>0.37381633013528409</v>
+      </c>
+      <c r="C8" s="101">
+        <f t="shared" ref="C8:F8" si="2">C7/C6</f>
+        <v>0.35841207096177363</v>
+      </c>
+      <c r="D8" s="101">
+        <f t="shared" si="2"/>
+        <v>0.38744949646660287</v>
+      </c>
+      <c r="E8" s="101">
+        <f t="shared" si="2"/>
+        <v>0.42506067422029531</v>
+      </c>
+      <c r="F8" s="101">
+        <f t="shared" si="2"/>
+        <v>0.37531931175736638</v>
+      </c>
+      <c r="G8" s="62"/>
+      <c r="H8" s="66">
+        <f>AVERAGE(B8:F8)</f>
+        <v>0.38401157670826447</v>
+      </c>
       <c r="I8" s="63"/>
       <c r="J8" s="63"/>
       <c r="K8" s="63"/>
@@ -3376,980 +3601,1252 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="11">
+        <f>ABS(SUM(income_statement!B6:B8))</f>
+        <v>1353475</v>
+      </c>
+      <c r="C9" s="11">
+        <f>ABS(SUM(income_statement!C6:C8))</f>
+        <v>1317980</v>
+      </c>
+      <c r="D9" s="11">
+        <f>ABS(SUM(income_statement!D6:D8))</f>
+        <v>1368440</v>
+      </c>
+      <c r="E9" s="11">
+        <f>ABS(SUM(income_statement!E6:E8))</f>
+        <v>1532770</v>
+      </c>
+      <c r="F9" s="11">
+        <f>ABS(SUM(income_statement!F6:F8))</f>
+        <v>1561676</v>
+      </c>
+      <c r="G9" s="62">
+        <f t="shared" si="1"/>
+        <v>3.6418542769312889E-2</v>
+      </c>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="101">
+        <f>B9/B6</f>
+        <v>0.42014556830588029</v>
+      </c>
+      <c r="C10" s="101">
+        <f t="shared" ref="C10:F10" si="3">C9/C6</f>
+        <v>0.40900431385071612</v>
+      </c>
+      <c r="D10" s="101">
+        <f t="shared" si="3"/>
+        <v>0.39716144094224698</v>
+      </c>
+      <c r="E10" s="101">
+        <f t="shared" si="3"/>
+        <v>0.38362225282873141</v>
+      </c>
+      <c r="F10" s="101">
+        <f t="shared" si="3"/>
+        <v>0.36170931761493774</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="66">
+        <f t="shared" ref="H10:H17" si="4">AVERAGE(B10:F10)</f>
+        <v>0.39432857870850252</v>
+      </c>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B11" s="11">
         <f>income_statement!B9</f>
         <v>728104</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C11" s="11">
         <f>income_statement!C9</f>
         <v>780801</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D11" s="11">
         <f>income_statement!D9</f>
         <v>794644</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E11" s="11">
         <f>income_statement!E9</f>
         <v>883676</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F11" s="11">
         <f>income_statement!F9</f>
         <v>1243215</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="66">
+        <f>B11/B6</f>
+        <v>0.22601796772440177</v>
+      </c>
+      <c r="C12" s="66">
+        <f t="shared" ref="C12:F12" si="5">C11/C6</f>
+        <v>0.24230335608958634</v>
+      </c>
+      <c r="D12" s="66">
+        <f t="shared" si="5"/>
+        <v>0.23062900534631472</v>
+      </c>
+      <c r="E12" s="66">
+        <f t="shared" si="5"/>
+        <v>0.22116676206520355</v>
+      </c>
+      <c r="F12" s="66">
+        <f t="shared" si="5"/>
+        <v>0.28794862013545375</v>
+      </c>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66">
+        <f t="shared" si="4"/>
+        <v>0.24161314227219205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" s="11">
+        <f>SUM(income_statement!B10:B11)</f>
+        <v>-259866</v>
+      </c>
+      <c r="C13" s="11">
+        <f>SUM(income_statement!C10:C11)</f>
+        <v>-256911</v>
+      </c>
+      <c r="D13" s="11">
+        <f>SUM(income_statement!D10:D11)</f>
+        <v>-249048</v>
+      </c>
+      <c r="E13" s="11">
+        <f>SUM(income_statement!E10:E11)</f>
+        <v>-388900</v>
+      </c>
+      <c r="F13" s="11">
+        <f>SUM(income_statement!F10:F11)</f>
+        <v>-258425</v>
+      </c>
+      <c r="G13" s="62">
         <f t="shared" si="1"/>
-        <v>0.1431104793723732</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+        <v>-1.3891834624155663E-3</v>
+      </c>
+      <c r="H13" s="66"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="66">
+        <f>ABS(B13)/B11</f>
+        <v>0.35690780437959413</v>
+      </c>
+      <c r="C14" s="66">
+        <f t="shared" ref="C14:F14" si="6">ABS(C13)/C11</f>
+        <v>0.32903518310043151</v>
+      </c>
+      <c r="D14" s="66">
+        <f t="shared" si="6"/>
+        <v>0.31340826835664776</v>
+      </c>
+      <c r="E14" s="66">
+        <f t="shared" si="6"/>
+        <v>0.44009342790796629</v>
+      </c>
+      <c r="F14" s="66">
+        <f t="shared" si="6"/>
+        <v>0.2078683091822412</v>
+      </c>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66">
+        <f>AVERAGE(B14:F14)</f>
+        <v>0.32946259858537613</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B15" s="11">
         <f>income_statement!B12</f>
         <v>468238</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C15" s="11">
         <f>income_statement!C12</f>
         <v>523890</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D15" s="11">
         <f>income_statement!D12</f>
         <v>545596</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E15" s="11">
         <f>income_statement!E12</f>
         <v>494776</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F15" s="11">
         <f>income_statement!F12</f>
         <v>984790</v>
       </c>
-      <c r="G10" s="62">
+      <c r="G15" s="62">
         <f t="shared" si="1"/>
         <v>0.20425717756209383</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="66">
+        <f>B15/B6</f>
+        <v>0.14535039111354756</v>
+      </c>
+      <c r="C16" s="66">
+        <f t="shared" ref="C16:F16" si="7">C15/C6</f>
+        <v>0.16257702695280024</v>
+      </c>
+      <c r="D16" s="66">
+        <f t="shared" si="7"/>
+        <v>0.15834796814791016</v>
+      </c>
+      <c r="E16" s="66">
+        <f t="shared" si="7"/>
+        <v>0.12383272360862256</v>
+      </c>
+      <c r="F16" s="66">
+        <f t="shared" si="7"/>
+        <v>0.2280932273365375</v>
+      </c>
+      <c r="G16" s="62"/>
+      <c r="H16" s="66">
+        <f t="shared" si="4"/>
+        <v>0.16364026743188359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="66">
+        <f>B15/B11</f>
+        <v>0.64309219562040587</v>
+      </c>
+      <c r="C17" s="66">
+        <f t="shared" ref="C17:F17" si="8">C15/C11</f>
+        <v>0.67096481689956855</v>
+      </c>
+      <c r="D17" s="66">
+        <f t="shared" si="8"/>
+        <v>0.6865917316433523</v>
+      </c>
+      <c r="E17" s="66">
+        <f t="shared" si="8"/>
+        <v>0.55990657209203376</v>
+      </c>
+      <c r="F17" s="66">
+        <f t="shared" si="8"/>
+        <v>0.7921316908177588</v>
+      </c>
+      <c r="G17" s="62"/>
+      <c r="H17" s="66">
+        <f t="shared" si="4"/>
+        <v>0.67053740141462392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="11">
-        <f>B10*(1-$B$1)</f>
+      <c r="B18" s="11">
+        <f>B15*(1-$B$1)</f>
         <v>374590.4</v>
       </c>
-      <c r="C11" s="11">
-        <f>C10*(1-$B$1)</f>
+      <c r="C18" s="11">
+        <f>C15*(1-$B$1)</f>
         <v>419112</v>
       </c>
-      <c r="D11" s="11">
-        <f>D10*(1-$B$1)</f>
+      <c r="D18" s="11">
+        <f>D15*(1-$B$1)</f>
         <v>436476.80000000005</v>
       </c>
-      <c r="E11" s="11">
-        <f>E10*(1-$B$1)</f>
+      <c r="E18" s="11">
+        <f>E15*(1-$B$1)</f>
         <v>395820.80000000005</v>
       </c>
-      <c r="F11" s="11">
-        <f>F10*(1-$B$1)</f>
+      <c r="F18" s="11">
+        <f>F15*(1-$B$1)</f>
         <v>787832</v>
       </c>
-      <c r="G11" s="62">
+      <c r="G18" s="62">
         <f t="shared" si="1"/>
         <v>0.20425717756209383</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="66">
+        <f>B18/B6</f>
+        <v>0.11628031289083805</v>
+      </c>
+      <c r="C19" s="66">
+        <f>C18/C6</f>
+        <v>0.13006162156224019</v>
+      </c>
+      <c r="D19" s="66">
+        <f>D18/D6</f>
+        <v>0.12667837451832814</v>
+      </c>
+      <c r="E19" s="66">
+        <f>E18/E6</f>
+        <v>9.906617888689806E-2</v>
+      </c>
+      <c r="F19" s="66">
+        <f>F18/F6</f>
+        <v>0.18247458186923002</v>
+      </c>
+      <c r="G19" s="62"/>
+      <c r="H19" s="102">
+        <f>AVERAGE(B19:F19)</f>
+        <v>0.13091221394550689</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B20" s="11">
         <f>income_statement!B19</f>
         <v>385910</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C20" s="11">
         <f>income_statement!C19</f>
         <v>560472</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D20" s="11">
         <f>income_statement!D19</f>
         <v>542300</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E20" s="11">
         <f>income_statement!E19</f>
         <v>458779</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F20" s="11">
         <f>income_statement!F19</f>
         <v>966813</v>
       </c>
-      <c r="G12" s="62">
+      <c r="G20" s="62">
         <f t="shared" si="1"/>
         <v>0.25809695791895071</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="62"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="64" t="s">
+        <v>199</v>
+      </c>
+      <c r="B21" s="66">
+        <f>B20/B11</f>
+        <v>0.53002043664091947</v>
+      </c>
+      <c r="C21" s="66">
+        <f>C20/C11</f>
+        <v>0.71781670361590211</v>
+      </c>
+      <c r="D21" s="66">
+        <f>D20/D11</f>
+        <v>0.68244396232778448</v>
+      </c>
+      <c r="E21" s="66">
+        <f>E20/E11</f>
+        <v>0.51917105364409577</v>
+      </c>
+      <c r="F21" s="66">
+        <f>F20/F11</f>
+        <v>0.77767160145268521</v>
+      </c>
+      <c r="G21" s="62"/>
+      <c r="H21" s="102">
+        <f>AVERAGE(B21:F21)</f>
+        <v>0.64542475153627743</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B22" s="11">
         <f>cash_flow_statement!B7</f>
         <v>575479</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C22" s="11">
         <f>cash_flow_statement!C7</f>
         <v>588810</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D22" s="11">
         <f>cash_flow_statement!D7</f>
         <v>591657</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E22" s="11">
         <f>cash_flow_statement!E7</f>
         <v>394715</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F22" s="11">
         <f>cash_flow_statement!F7</f>
         <v>818804</v>
       </c>
-      <c r="G14" s="62">
+      <c r="G22" s="62">
         <f t="shared" si="1"/>
         <v>9.2163400593102907E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B23" s="11">
         <f>SUM(cash_flow_statement!B10,cash_flow_statement!B11)</f>
         <v>-257084</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C23" s="11">
         <f>SUM(cash_flow_statement!C10,cash_flow_statement!C11)</f>
         <v>-228139</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D23" s="11">
         <f>SUM(cash_flow_statement!D10,cash_flow_statement!D11)</f>
         <v>-214447</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E23" s="11">
         <f>SUM(cash_flow_statement!E10,cash_flow_statement!E11)</f>
         <v>-266738</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F23" s="11">
         <f>SUM(cash_flow_statement!F10,cash_flow_statement!F11)</f>
         <v>-303704</v>
       </c>
-      <c r="G15" s="62">
+      <c r="G23" s="62">
         <f t="shared" si="1"/>
         <v>4.2542734085359024E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="74" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="B16" s="67">
-        <f>ABS(B15)/B6</f>
+      <c r="B24" s="66">
+        <f>ABS(B23)/B6</f>
         <v>7.9803988461071632E-2</v>
       </c>
-      <c r="C16" s="67">
-        <f t="shared" ref="C16:F16" si="2">ABS(C15)/C6</f>
+      <c r="C24" s="66">
+        <f>ABS(C23)/C6</f>
         <v>7.0797610857212187E-2</v>
       </c>
-      <c r="D16" s="67">
-        <f t="shared" si="2"/>
+      <c r="D24" s="66">
+        <f>ABS(D23)/D6</f>
         <v>6.2238811731418285E-2</v>
       </c>
-      <c r="E16" s="67">
-        <f t="shared" si="2"/>
+      <c r="E24" s="66">
+        <f>ABS(E23)/E6</f>
         <v>6.6759287091364097E-2</v>
       </c>
-      <c r="F16" s="67">
-        <f t="shared" si="2"/>
+      <c r="F24" s="66">
+        <f>ABS(F23)/F6</f>
         <v>7.0342738568644883E-2</v>
       </c>
-      <c r="G16" s="62"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+      <c r="G24" s="62"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B25" s="13">
         <f>SUM(cash_flow_statement!B22,cash_flow_statement!B23,cash_flow_statement!B24)</f>
         <v>98267</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C25" s="13">
         <f>SUM(cash_flow_statement!C22,cash_flow_statement!C23,cash_flow_statement!C24)</f>
         <v>-27250</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D25" s="13">
         <f>SUM(cash_flow_statement!D22,cash_flow_statement!D23,cash_flow_statement!D24)</f>
         <v>-112410</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E25" s="13">
         <f>SUM(cash_flow_statement!E22,cash_flow_statement!E23,cash_flow_statement!E24)</f>
         <v>63421</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F25" s="13">
         <f>SUM(cash_flow_statement!F22,cash_flow_statement!F23,cash_flow_statement!F24)</f>
         <v>-595465</v>
       </c>
-      <c r="G17" s="62" t="e">
-        <f>(F17/B17)^(1/4)-1</f>
+      <c r="G25" s="62" t="e">
+        <f>(F25/B25)^(1/4)-1</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="4" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="14">
-        <f>SUM(B14:B17)</f>
+      <c r="B26" s="14">
+        <f>SUM(B22:B25)</f>
         <v>416662.07980398845</v>
       </c>
-      <c r="C18" s="14">
-        <f t="shared" ref="C18:F18" si="3">SUM(C14:C17)</f>
+      <c r="C26" s="14">
+        <f t="shared" ref="C26:F26" si="9">SUM(C22:C25)</f>
         <v>333421.07079761085</v>
       </c>
-      <c r="D18" s="14">
-        <f t="shared" si="3"/>
+      <c r="D26" s="14">
+        <f t="shared" si="9"/>
         <v>264800.06223881175</v>
       </c>
-      <c r="E18" s="14">
-        <f t="shared" si="3"/>
+      <c r="E26" s="14">
+        <f t="shared" si="9"/>
         <v>191398.06675928709</v>
       </c>
-      <c r="F18" s="14">
-        <f t="shared" si="3"/>
+      <c r="F26" s="14">
+        <f t="shared" si="9"/>
         <v>-80364.929657261411</v>
       </c>
-      <c r="G18" s="62" t="e">
+      <c r="G26" s="62" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="G19" s="62"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" s="62"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>137</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B28" s="11">
         <f>SUM(balance_sheet!B30,balance_sheet!B40,balance_sheet!B41)</f>
         <v>1275779</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C28" s="11">
         <f>SUM(balance_sheet!C30,balance_sheet!C40,balance_sheet!C41)</f>
         <v>1232168</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D28" s="11">
         <f>SUM(balance_sheet!D30,balance_sheet!D40,balance_sheet!D41)</f>
         <v>1137062</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E28" s="11">
         <f>SUM(balance_sheet!E30,balance_sheet!E40,balance_sheet!E41)</f>
         <v>1214722</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F28" s="11">
         <f>SUM(balance_sheet!F30,balance_sheet!F40,balance_sheet!F41)</f>
         <v>608888</v>
       </c>
-      <c r="G20" s="62">
+      <c r="G28" s="62">
         <f t="shared" si="1"/>
         <v>-0.16882879058056532</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B29" s="13">
         <f>balance_sheet!B22</f>
         <v>837403</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C29" s="13">
         <f>balance_sheet!C22</f>
         <v>1218279</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D29" s="13">
         <f>balance_sheet!D22</f>
         <v>1203611</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E29" s="13">
         <f>balance_sheet!E22</f>
         <v>1341488</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F29" s="13">
         <f>balance_sheet!F22</f>
         <v>1120712</v>
       </c>
-      <c r="G21" s="62">
+      <c r="G29" s="62">
         <f t="shared" si="1"/>
         <v>7.5572964823968469E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="4" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B22" s="14">
-        <f>B20-B21</f>
+      <c r="B30" s="14">
+        <f>B28-B29</f>
         <v>438376</v>
       </c>
-      <c r="C22" s="14">
-        <f t="shared" ref="C22:F22" si="4">C20-C21</f>
+      <c r="C30" s="14">
+        <f t="shared" ref="C30:F30" si="10">C28-C29</f>
         <v>13889</v>
       </c>
-      <c r="D22" s="14">
-        <f t="shared" si="4"/>
+      <c r="D30" s="14">
+        <f t="shared" si="10"/>
         <v>-66549</v>
       </c>
-      <c r="E22" s="14">
-        <f t="shared" si="4"/>
+      <c r="E30" s="14">
+        <f t="shared" si="10"/>
         <v>-126766</v>
       </c>
-      <c r="F22" s="14">
-        <f t="shared" si="4"/>
+      <c r="F30" s="14">
+        <f t="shared" si="10"/>
         <v>-511824</v>
       </c>
-      <c r="G22" s="62" t="e">
+      <c r="G30" s="62" t="e">
         <f t="shared" si="1"/>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B31" s="13">
         <f>balance_sheet!B61</f>
         <v>3690821</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C31" s="13">
         <f>balance_sheet!C61</f>
         <v>3603007</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D31" s="13">
         <f>balance_sheet!D61</f>
         <v>4375204</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E31" s="13">
         <f>balance_sheet!E61</f>
         <v>4911457</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F31" s="13">
         <f>balance_sheet!F61</f>
         <v>5632028</v>
       </c>
-      <c r="G23" s="62">
+      <c r="G31" s="62">
         <f t="shared" si="1"/>
         <v>0.11143854859117819</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="4" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="14">
-        <f>SUM(B22:B23)</f>
+      <c r="B32" s="14">
+        <f>SUM(B30:B31)</f>
         <v>4129197</v>
       </c>
-      <c r="C24" s="14">
-        <f t="shared" ref="C24:F24" si="5">SUM(C22:C23)</f>
+      <c r="C32" s="14">
+        <f t="shared" ref="C32:F32" si="11">SUM(C30:C31)</f>
         <v>3616896</v>
       </c>
-      <c r="D24" s="14">
-        <f t="shared" si="5"/>
+      <c r="D32" s="14">
+        <f t="shared" si="11"/>
         <v>4308655</v>
       </c>
-      <c r="E24" s="14">
-        <f t="shared" si="5"/>
+      <c r="E32" s="14">
+        <f t="shared" si="11"/>
         <v>4784691</v>
       </c>
-      <c r="F24" s="14">
-        <f t="shared" si="5"/>
+      <c r="F32" s="14">
+        <f t="shared" si="11"/>
         <v>5120204</v>
       </c>
-      <c r="G24" s="62">
+      <c r="G32" s="62">
         <f t="shared" si="1"/>
         <v>5.5250132489215842E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="G25" s="62"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" s="62"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="56">
+      <c r="B34" s="56">
         <v>385671</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C34" s="56">
         <v>560246</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D34" s="56">
         <v>541903</v>
       </c>
-      <c r="E26" s="56">
+      <c r="E34" s="56">
         <v>458786</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F34" s="56">
         <v>966545</v>
       </c>
-      <c r="G26" s="62">
+      <c r="G34" s="62">
         <f t="shared" si="1"/>
         <v>0.25820461454614518</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="55">
+      <c r="B35" s="55">
         <v>17.899999999999999</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C35" s="55">
         <v>17.489999999999998</v>
       </c>
-      <c r="D27" s="55">
+      <c r="D35" s="55">
         <v>22.71</v>
       </c>
-      <c r="E27" s="55">
+      <c r="E35" s="55">
         <v>25.5</v>
       </c>
-      <c r="F27" s="55">
+      <c r="F35" s="55">
         <v>29.24</v>
       </c>
-      <c r="G27" s="62">
+      <c r="G35" s="62">
         <f t="shared" si="1"/>
         <v>0.13052737852370599</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="10" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="61">
+      <c r="B36" s="61">
         <v>191409874</v>
       </c>
-      <c r="C28" s="61">
+      <c r="C36" s="61">
         <v>192288607</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D36" s="61">
         <v>192131838</v>
       </c>
-      <c r="E28" s="61">
+      <c r="E36" s="61">
         <v>186377503</v>
       </c>
-      <c r="F28" s="61">
+      <c r="F36" s="61">
         <v>185131838</v>
       </c>
-      <c r="G28" s="62">
+      <c r="G36" s="62">
         <f t="shared" si="1"/>
         <v>-8.3025560326389636E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="4" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="58">
+      <c r="B37" s="58">
         <v>1.8779999999999999</v>
       </c>
-      <c r="C29" s="58">
+      <c r="C37" s="58">
         <v>2.7490000000000001</v>
       </c>
-      <c r="D29" s="58">
-        <f>D26/D28 *1000</f>
+      <c r="D37" s="58">
+        <f>D34/D36 *1000</f>
         <v>2.8204747617102379</v>
       </c>
-      <c r="E29" s="58">
-        <f>E26/E28 *1000</f>
+      <c r="E37" s="58">
+        <f>E34/E36 *1000</f>
         <v>2.4615953782791045</v>
       </c>
-      <c r="F29" s="58">
-        <f>F26/F28 *1000</f>
+      <c r="F37" s="58">
+        <f>F34/F36 *1000</f>
         <v>5.2208469944537574</v>
       </c>
-      <c r="G29" s="62">
+      <c r="G37" s="62">
         <f t="shared" si="1"/>
         <v>0.29125300268040122</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="62"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="10" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="62"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="60">
+      <c r="B39" s="60">
         <v>26559</v>
       </c>
-      <c r="C31" s="60">
+      <c r="C39" s="60">
         <v>31802</v>
       </c>
-      <c r="D31" s="60">
+      <c r="D39" s="60">
         <v>48033</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E39" s="60">
         <v>74053</v>
       </c>
-      <c r="F31" s="60">
+      <c r="F39" s="60">
         <v>83309</v>
       </c>
-      <c r="G31" s="62">
+      <c r="G39" s="62">
         <f t="shared" si="1"/>
         <v>0.33082224204857358</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="4" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="59">
-        <f>B31/B28*1000</f>
+      <c r="B40" s="59">
+        <f>B39/B36*1000</f>
         <v>0.13875459737254725</v>
       </c>
-      <c r="C32" s="59">
+      <c r="C40" s="59">
         <v>0.25</v>
       </c>
-      <c r="D32" s="59">
+      <c r="D40" s="59">
         <v>0.4</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E40" s="59">
         <v>0.45</v>
       </c>
-      <c r="F32" s="59">
+      <c r="F40" s="59">
         <v>0.6</v>
       </c>
-      <c r="G32" s="62">
+      <c r="G40" s="62">
         <f t="shared" si="1"/>
         <v>0.44203555059449395</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="62"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="62"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="62"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="62"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B43" s="11">
         <f>(balance_sheet!B23-balance_sheet!B22)-(balance_sheet!B47-balance_sheet!B41-balance_sheet!B40)</f>
         <v>519817</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C43" s="11">
         <f>(balance_sheet!C23-balance_sheet!C22)-(balance_sheet!C47-balance_sheet!C41-balance_sheet!C40)</f>
         <v>334240</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D43" s="11">
         <f>(balance_sheet!D23-balance_sheet!D22)-(balance_sheet!D47-balance_sheet!D41-balance_sheet!D40)</f>
         <v>505980</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E43" s="11">
         <f>(balance_sheet!E23-balance_sheet!E22)-(balance_sheet!E47-balance_sheet!E41-balance_sheet!E40)</f>
         <v>799631</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F43" s="11">
         <f>(balance_sheet!F23-balance_sheet!F22)-(balance_sheet!F47-balance_sheet!F41-balance_sheet!F40)</f>
         <v>1014099</v>
       </c>
-      <c r="G35" s="62">
+      <c r="G43" s="62">
         <f t="shared" si="1"/>
         <v>0.18183669139552849</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="67">
-        <f>B35/B6</f>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="66">
+        <f>B43/B6</f>
         <v>0.16136153891284125</v>
       </c>
-      <c r="C36" s="67">
-        <f t="shared" ref="C36:F36" si="6">C35/C6</f>
+      <c r="C44" s="66">
+        <f>C43/C6</f>
         <v>0.10372357840138952</v>
       </c>
-      <c r="D36" s="67">
-        <f t="shared" si="6"/>
+      <c r="D44" s="66">
+        <f>D43/D6</f>
         <v>0.14685024253014975</v>
       </c>
-      <c r="E36" s="67">
-        <f t="shared" si="6"/>
+      <c r="E44" s="66">
+        <f>E43/E6</f>
         <v>0.20013194781453925</v>
       </c>
-      <c r="F36" s="67">
-        <f t="shared" si="6"/>
+      <c r="F44" s="66">
+        <f>F43/F6</f>
         <v>0.2348816638560052</v>
       </c>
-      <c r="G36" s="62"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+      <c r="G44" s="62"/>
+      <c r="H44" s="98">
+        <f>AVERAGE(B44:F44)</f>
+        <v>0.16938979430298501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B45" s="11">
         <v>0</v>
       </c>
-      <c r="C37" s="11">
-        <f>C35-B35</f>
+      <c r="C45" s="11">
+        <f>C43-B43</f>
         <v>-185577</v>
       </c>
-      <c r="D37" s="11">
-        <f t="shared" ref="D37:F37" si="7">D35-C35</f>
+      <c r="D45" s="11">
+        <f t="shared" ref="D45:F45" si="12">D43-C43</f>
         <v>171740</v>
       </c>
-      <c r="E37" s="11">
-        <f t="shared" si="7"/>
+      <c r="E45" s="11">
+        <f t="shared" si="12"/>
         <v>293651</v>
       </c>
-      <c r="F37" s="11">
-        <f t="shared" si="7"/>
+      <c r="F45" s="11">
+        <f t="shared" si="12"/>
         <v>214468</v>
       </c>
-      <c r="G37" s="62"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+      <c r="G45" s="62"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
         <v>146</v>
       </c>
-      <c r="B38" s="56">
-        <f>SUM(B26,B22)</f>
+      <c r="B46" s="56">
+        <f>SUM(B34,B30)</f>
         <v>824047</v>
       </c>
-      <c r="C38" s="56">
-        <f>SUM(C26,C22)</f>
+      <c r="C46" s="56">
+        <f>SUM(C34,C30)</f>
         <v>574135</v>
       </c>
-      <c r="D38" s="56">
-        <f>SUM(D26,D22)</f>
+      <c r="D46" s="56">
+        <f>SUM(D34,D30)</f>
         <v>475354</v>
       </c>
-      <c r="E38" s="56">
-        <f>SUM(E26,E22)</f>
+      <c r="E46" s="56">
+        <f>SUM(E34,E30)</f>
         <v>332020</v>
       </c>
-      <c r="F38" s="56">
-        <f>SUM(F26,F22)</f>
+      <c r="F46" s="56">
+        <f>SUM(F34,F30)</f>
         <v>454721</v>
       </c>
-      <c r="G38" s="62">
+      <c r="G46" s="62">
         <f t="shared" si="1"/>
         <v>-0.13811711409158478</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A40" s="57" t="s">
+    <row r="48" spans="1:12" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A48" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="B40" s="57">
+      <c r="B48" s="57">
         <v>2019</v>
       </c>
-      <c r="C40" s="57">
+      <c r="C48" s="57">
         <v>2020</v>
       </c>
-      <c r="D40" s="57">
+      <c r="D48" s="57">
         <v>2021</v>
       </c>
-      <c r="E40" s="57">
+      <c r="E48" s="57">
         <v>2022</v>
       </c>
-      <c r="F40" s="57">
+      <c r="F48" s="57">
         <v>2023</v>
       </c>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57" t="s">
+      <c r="G48" s="57"/>
+      <c r="H48" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="I40" s="57" t="s">
+      <c r="I48" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="J40" s="57" t="s">
+      <c r="J48" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="K40" s="57" t="s">
+      <c r="K48" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="L40" s="57" t="s">
+      <c r="L48" s="57" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="52">
-        <f>B10/B6</f>
+      <c r="B49" s="52">
+        <f>B15/B6</f>
         <v>0.14535039111354756</v>
       </c>
-      <c r="C41" s="52">
-        <f>C10/C6</f>
+      <c r="C49" s="52">
+        <f>C15/C6</f>
         <v>0.16257702695280024</v>
       </c>
-      <c r="D41" s="52">
-        <f>D10/D6</f>
+      <c r="D49" s="52">
+        <f>D15/D6</f>
         <v>0.15834796814791016</v>
       </c>
-      <c r="E41" s="52">
-        <f>E10/E6</f>
+      <c r="E49" s="52">
+        <f>E15/E6</f>
         <v>0.12383272360862256</v>
       </c>
-      <c r="F41" s="52">
-        <f>F10/F6</f>
+      <c r="F49" s="52">
+        <f>F15/F6</f>
         <v>0.2280932273365375</v>
       </c>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52">
-        <f>H10/H6</f>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52">
+        <f>H15/H6</f>
         <v>0</v>
       </c>
-      <c r="I41" s="52">
-        <f>I10/I6</f>
+      <c r="I49" s="52">
+        <f>I15/I6</f>
         <v>0</v>
       </c>
-      <c r="J41" s="52">
-        <f>J10/J6</f>
+      <c r="J49" s="52">
+        <f>J15/J6</f>
         <v>0</v>
       </c>
-      <c r="K41" s="52">
-        <f>K10/K6</f>
+      <c r="K49" s="52">
+        <f>K15/K6</f>
         <v>0</v>
       </c>
-      <c r="L41" s="52">
-        <f>L10/L6</f>
+      <c r="L49" s="52">
+        <f>L15/L6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
         <v>125</v>
       </c>
-      <c r="B42" s="52">
-        <f>B11/B24</f>
+      <c r="B50" s="52">
+        <f>B18/B32</f>
         <v>9.0717493013774839E-2</v>
       </c>
-      <c r="C42" s="52">
-        <f>C11/C24</f>
+      <c r="C50" s="52">
+        <f>C18/C32</f>
         <v>0.11587615458116574</v>
       </c>
-      <c r="D42" s="52">
-        <f>D11/D24</f>
+      <c r="D50" s="52">
+        <f>D18/D32</f>
         <v>0.10130233216630249</v>
       </c>
-      <c r="E42" s="52">
-        <f>E11/E24</f>
+      <c r="E50" s="52">
+        <f>E18/E32</f>
         <v>8.2726512537591251E-2</v>
       </c>
-      <c r="F42" s="52">
-        <f>F11/F24</f>
+      <c r="F50" s="52">
+        <f>F18/F32</f>
         <v>0.15386730684949271</v>
       </c>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="52"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" s="52">
-        <f>B12/B6</f>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="52"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>165</v>
+      </c>
+      <c r="B51" s="52">
+        <f>B20/B6</f>
         <v>0.11979414194198065</v>
       </c>
-      <c r="C43" s="52">
-        <f t="shared" ref="C43:F43" si="8">C12/C6</f>
+      <c r="C51" s="52">
+        <f>C20/C6</f>
         <v>0.17392939634329699</v>
       </c>
-      <c r="D43" s="52">
-        <f t="shared" si="8"/>
+      <c r="D51" s="52">
+        <f>D20/D6</f>
         <v>0.15739137223625482</v>
       </c>
-      <c r="E43" s="52">
-        <f t="shared" si="8"/>
+      <c r="E51" s="52">
+        <f>E20/E6</f>
         <v>0.11482338089244476</v>
       </c>
-      <c r="F43" s="52">
-        <f t="shared" si="8"/>
+      <c r="F51" s="52">
+        <f>F20/F6</f>
         <v>0.22392946455682922</v>
       </c>
-      <c r="G43" s="52"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="52"/>
-      <c r="K43" s="52"/>
-      <c r="L43" s="52"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="52">
-        <f>B38/B9</f>
+      <c r="B52" s="52">
+        <f>B46/B11</f>
         <v>1.1317710107347303</v>
       </c>
-      <c r="C44" s="52">
-        <f>C38/C9</f>
+      <c r="C52" s="52">
+        <f>C46/C11</f>
         <v>0.73531540046695631</v>
       </c>
-      <c r="D44" s="52">
-        <f>D38/D9</f>
+      <c r="D52" s="52">
+        <f>D46/D11</f>
         <v>0.59819743180594076</v>
       </c>
-      <c r="E44" s="52">
-        <f>E38/E9</f>
+      <c r="E52" s="52">
+        <f>E46/E11</f>
         <v>0.37572594480329896</v>
       </c>
-      <c r="F44" s="52">
-        <f>F38/F9</f>
+      <c r="F52" s="52">
+        <f>F46/F11</f>
         <v>0.36576215698813158</v>
       </c>
-      <c r="G44" s="52"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
+      <c r="G52" s="52"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="53">
-        <f>B27/B29</f>
+      <c r="B53" s="53">
+        <f>B35/B37</f>
         <v>9.531416400425984</v>
       </c>
-      <c r="C45" s="53">
-        <f>C27/C29</f>
+      <c r="C53" s="53">
+        <f>C35/C37</f>
         <v>6.3623135685703884</v>
       </c>
-      <c r="D45" s="53">
-        <f>D27/D29</f>
+      <c r="D53" s="53">
+        <f>D35/D37</f>
         <v>8.0518359207828709</v>
       </c>
-      <c r="E45" s="53">
-        <f>E27/E29</f>
+      <c r="E53" s="53">
+        <f>E35/E37</f>
         <v>10.359135471657812</v>
       </c>
-      <c r="F45" s="53">
-        <f>F27/F29</f>
+      <c r="F53" s="53">
+        <f>F35/F37</f>
         <v>5.6006238127764361</v>
       </c>
-      <c r="G45" s="53"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
+      <c r="G53" s="53"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="52">
-        <f>B18/B26</f>
+      <c r="B54" s="52">
+        <f>B26/B34</f>
         <v>1.0803562616945233</v>
       </c>
-      <c r="C46" s="52">
-        <f t="shared" ref="C46:F46" si="9">C18/C26</f>
+      <c r="C54" s="52">
+        <f t="shared" ref="C54:F54" si="13">C26/C34</f>
         <v>0.59513333570897575</v>
       </c>
-      <c r="D46" s="52">
-        <f t="shared" si="9"/>
+      <c r="D54" s="52">
+        <f t="shared" si="13"/>
         <v>0.48864845228539378</v>
       </c>
-      <c r="E46" s="52">
-        <f t="shared" si="9"/>
+      <c r="E54" s="52">
+        <f t="shared" si="13"/>
         <v>0.41718375617234854</v>
       </c>
-      <c r="F46" s="52">
-        <f t="shared" si="9"/>
+      <c r="F54" s="52">
+        <f t="shared" si="13"/>
         <v>-8.3146599131195556E-2</v>
       </c>
-      <c r="G46" s="52"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
+      <c r="G54" s="52"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
         <v>129</v>
       </c>
-      <c r="B47" s="52">
-        <f>B32/B27</f>
+      <c r="B55" s="52">
+        <f>B40/B35</f>
         <v>7.7516534844998472E-3</v>
       </c>
-      <c r="C47" s="52">
-        <f>C32/C27</f>
+      <c r="C55" s="52">
+        <f>C40/C35</f>
         <v>1.4293882218410521E-2</v>
       </c>
-      <c r="D47" s="52">
-        <f>D32/D27</f>
+      <c r="D55" s="52">
+        <f>D40/D35</f>
         <v>1.7613386173491855E-2</v>
       </c>
-      <c r="E47" s="52">
-        <f>E32/E27</f>
+      <c r="E55" s="52">
+        <f>E40/E35</f>
         <v>1.7647058823529412E-2</v>
       </c>
-      <c r="F47" s="52">
-        <f>F32/F27</f>
+      <c r="F55" s="52">
+        <f>F40/F35</f>
         <v>2.0519835841313269E-2</v>
       </c>
-      <c r="G47" s="52"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
+      <c r="G55" s="52"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
         <v>120</v>
       </c>
-      <c r="B48" s="52">
-        <f>B22/B21</f>
+      <c r="B56" s="52">
+        <f>B30/B29</f>
         <v>0.52349466147123902</v>
       </c>
-      <c r="C48" s="52">
-        <f>C22/C21</f>
+      <c r="C56" s="52">
+        <f>C30/C29</f>
         <v>1.1400508422126622E-2</v>
       </c>
-      <c r="D48" s="52">
-        <f>D22/D21</f>
+      <c r="D56" s="52">
+        <f>D30/D29</f>
         <v>-5.5291119805319158E-2</v>
       </c>
-      <c r="E48" s="52">
-        <f>E22/E21</f>
+      <c r="E56" s="52">
+        <f>E30/E29</f>
         <v>-9.4496559044881509E-2</v>
       </c>
-      <c r="F48" s="52">
-        <f>F22/F21</f>
+      <c r="F56" s="52">
+        <f>F30/F29</f>
         <v>-0.4566953865042937</v>
       </c>
-      <c r="G48" s="52"/>
+      <c r="G56" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G17" evalError="1"/>
+    <ignoredError sqref="G25" evalError="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4359,7 +4856,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4369,7 +4866,7 @@
     <col min="3" max="6" width="13.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -4388,8 +4885,11 @@
       <c r="F1" s="30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>3</v>
       </c>
@@ -4408,8 +4908,9 @@
       <c r="F2" s="33">
         <v>4317489</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="99"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4428,8 +4929,9 @@
       <c r="F3" s="11">
         <v>50372</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="99"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4448,8 +4950,9 @@
       <c r="F4" s="11">
         <v>57467</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="99"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -4468,8 +4971,9 @@
       <c r="F5" s="11">
         <v>-1620437</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="99"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -4488,8 +4992,9 @@
       <c r="F6" s="11">
         <v>-886919</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="99"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -4508,8 +5013,9 @@
       <c r="F7" s="11">
         <v>-589300</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="99"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
@@ -4528,8 +5034,9 @@
       <c r="F8" s="13">
         <v>-85457</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="99"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="32" t="s">
         <v>10</v>
       </c>
@@ -4553,8 +5060,9 @@
         <f>SUM(F2:F8)</f>
         <v>1243215</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" s="100"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4573,8 +5081,9 @@
       <c r="F10" s="11">
         <v>-248237</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="99"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -4593,8 +5102,9 @@
       <c r="F11" s="13">
         <v>-10188</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" s="99"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="32" t="s">
         <v>9</v>
       </c>
@@ -4618,8 +5128,9 @@
         <f>SUM(F9:F11)</f>
         <v>984790</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="99"/>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -4638,8 +5149,9 @@
       <c r="F13" s="11">
         <v>161236</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" s="99"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -4658,8 +5170,9 @@
       <c r="F14" s="11">
         <v>241</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" s="99"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -4678,8 +5191,9 @@
       <c r="F15" s="11">
         <v>98091</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" s="99"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
@@ -4698,6 +5212,7 @@
       <c r="F16" s="13">
         <v>-103489</v>
       </c>
+      <c r="G16" s="99"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="32" t="s">
@@ -4723,6 +5238,7 @@
         <f>SUM(F12:F16)</f>
         <v>1140869</v>
       </c>
+      <c r="G17" s="99"/>
     </row>
     <row r="18" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="5" t="s">
@@ -4743,6 +5259,7 @@
       <c r="F18" s="12">
         <v>-174056</v>
       </c>
+      <c r="G18" s="99"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="32" t="s">
@@ -4768,6 +5285,7 @@
         <f>SUM(F17:F18)</f>
         <v>966813</v>
       </c>
+      <c r="G19" s="99"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1"/>
@@ -6722,40 +7240,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5E1897-464E-4698-93F5-3EE1A720698F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA29763-84F2-4BF8-B8A9-16F52912B2DE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60B6CD0-0E5F-4E0E-B225-D14CF5F0CAFC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>